<commit_message>
GL Codes have been Updated with Dynamic wait and Working till Issue.
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -3,21 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr documentId="13_ncr:801_{C329D569-DBF2-4E71-8EAA-DEE823735EC5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\New folder\FCGA-Version2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{8F17B4BB-AF58-4C84-846A-88E45ED4E7FE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12930" windowWidth="24030" xWindow="2730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2730"/>
+    <workbookView windowHeight="13140" windowWidth="24240" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TD_GL" r:id="rId1" sheetId="3"/>
     <sheet name="TD_WC" r:id="rId2" sheetId="2"/>
     <sheet name="TD_CSQ" r:id="rId3" sheetId="4"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <oleSize ref="H1:N22"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="146">
   <si>
     <t>Class Code</t>
   </si>
@@ -356,149 +361,123 @@
     <t>0</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>$1,163</t>
+    <t>All Island Credit Corp.</t>
+  </si>
+  <si>
+    <t>AddressState</t>
+  </si>
+  <si>
+    <t>PT_Gross Annual Payroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Officers Gross Annual Payroll</t>
+  </si>
+  <si>
+    <t>ContactEmail</t>
+  </si>
+  <si>
+    <t>ContactPhone</t>
+  </si>
+  <si>
+    <t>Huntsville</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>35801</t>
+  </si>
+  <si>
+    <t>Siddharth</t>
+  </si>
+  <si>
+    <t>187200</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-290247362</t>
+  </si>
+  <si>
+    <t>FWAL0020283000</t>
+  </si>
+  <si>
+    <t>Referral Flow</t>
+  </si>
+  <si>
+    <t>Additional Insured</t>
+  </si>
+  <si>
+    <t>Raja Kumar</t>
+  </si>
+  <si>
+    <t>UW Rate Type</t>
+  </si>
+  <si>
+    <t>Modified Rates</t>
+  </si>
+  <si>
+    <t>IRPM</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>CTR</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>FCGA AUTM -020015449</t>
+  </si>
+  <si>
+    <t>03/09/2020</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>$1,221</t>
+  </si>
+  <si>
+    <t>$25</t>
+  </si>
+  <si>
+    <t>FCGA AUTM -995180704</t>
+  </si>
+  <si>
+    <t>FCGA AUTM -771357723</t>
+  </si>
+  <si>
+    <t>$1,548</t>
   </si>
   <si>
     <t>$90</t>
   </si>
   <si>
     <t>$100</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>$1,221</t>
-  </si>
-  <si>
-    <t>$25</t>
-  </si>
-  <si>
-    <t>All Island Credit Corp.</t>
-  </si>
-  <si>
-    <t>AddressState</t>
-  </si>
-  <si>
-    <t>PT_Gross Annual Payroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Officers Gross Annual Payroll</t>
-  </si>
-  <si>
-    <t>ContactEmail</t>
-  </si>
-  <si>
-    <t>ContactPhone</t>
-  </si>
-  <si>
-    <t>Huntsville</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Address 1</t>
-  </si>
-  <si>
-    <t>35801</t>
-  </si>
-  <si>
-    <t>Siddharth</t>
-  </si>
-  <si>
-    <t>187200</t>
-  </si>
-  <si>
-    <t>test@test.com</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-290247362</t>
-  </si>
-  <si>
-    <t>FWAL0020283000</t>
-  </si>
-  <si>
-    <t>$1,548</t>
-  </si>
-  <si>
-    <t>Referral Flow</t>
-  </si>
-  <si>
-    <t>Additional Insured</t>
-  </si>
-  <si>
-    <t>Raja Kumar</t>
-  </si>
-  <si>
-    <t>02/28/2020</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -532827663</t>
-  </si>
-  <si>
-    <t>Q-41347</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -845438658</t>
-  </si>
-  <si>
-    <t>Q-41348</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -877527294</t>
-  </si>
-  <si>
-    <t>Q-41350</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -140248648</t>
-  </si>
-  <si>
-    <t>Q-41352</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -960423635</t>
-  </si>
-  <si>
-    <t>Q-41363</t>
-  </si>
-  <si>
-    <t>FGTX0020288600</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -419192510</t>
-  </si>
-  <si>
-    <t>03/02/2020</t>
-  </si>
-  <si>
-    <t>Q-41424</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -614516209</t>
-  </si>
-  <si>
-    <t>03/03/2020</t>
-  </si>
-  <si>
-    <t>Q-41546</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0;[Red]0"/>
@@ -1152,7 +1131,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5480">
+  <cellStyleXfs count="5528">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
@@ -6786,18 +6765,62 @@
     <xf borderId="0" fillId="0" fontId="36" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="37" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -6812,9 +6835,6 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="2" numFmtId="166" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -6848,9 +6868,6 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="5">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="39" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="40" numFmtId="166" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -6890,8 +6907,25 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="39" fontId="40" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="2" numFmtId="166" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="39" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5480">
+  <cellStyles count="5528">
     <cellStyle name="20% - Accent1 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="20% - Accent1 2 10" xfId="38" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20% - Accent1 2 10 2" xfId="3904" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -10488,53 +10522,101 @@
     <cellStyle name="Check Cell 3 9" xfId="954" xr:uid="{00000000-0005-0000-0000-0000090E0000}"/>
     <cellStyle name="ColumnHeaderStyle" xfId="3008" xr:uid="{00000000-0005-0000-0000-00000A0E0000}"/>
     <cellStyle builtinId="3" name="Comma" xfId="5479"/>
+    <cellStyle name="Comma 10" xfId="5527" xr:uid="{2DB90E8E-B40C-4B4B-9530-BD8234A70FD7}"/>
     <cellStyle name="Comma 2" xfId="3582" xr:uid="{00000000-0005-0000-0000-00000C0E0000}"/>
     <cellStyle name="Comma 2 10" xfId="2965" xr:uid="{00000000-0005-0000-0000-00000D0E0000}"/>
+    <cellStyle name="Comma 2 10 2" xfId="5507" xr:uid="{36CA78E7-1B40-4684-BD15-76F58D6BF49E}"/>
     <cellStyle name="Comma 2 11" xfId="2961" xr:uid="{00000000-0005-0000-0000-00000E0E0000}"/>
+    <cellStyle name="Comma 2 11 2" xfId="5506" xr:uid="{0ED2D251-FAAB-4561-9702-67630FB654E1}"/>
     <cellStyle name="Comma 2 12" xfId="2957" xr:uid="{00000000-0005-0000-0000-00000F0E0000}"/>
+    <cellStyle name="Comma 2 12 2" xfId="5505" xr:uid="{CE3718A9-5E91-490A-AE45-6F2F27C94CDA}"/>
     <cellStyle name="Comma 2 13" xfId="2953" xr:uid="{00000000-0005-0000-0000-0000100E0000}"/>
+    <cellStyle name="Comma 2 13 2" xfId="5504" xr:uid="{8DE2CED4-6BC4-43F9-AF01-55BF8CD4E5CC}"/>
     <cellStyle name="Comma 2 14" xfId="2948" xr:uid="{00000000-0005-0000-0000-0000110E0000}"/>
+    <cellStyle name="Comma 2 14 2" xfId="5503" xr:uid="{9DC33D54-1E4B-42FD-9647-854F85777C06}"/>
     <cellStyle name="Comma 2 15" xfId="2943" xr:uid="{00000000-0005-0000-0000-0000120E0000}"/>
+    <cellStyle name="Comma 2 15 2" xfId="5502" xr:uid="{581E18C0-40AC-4AA4-B9CE-5E09AD984DDA}"/>
     <cellStyle name="Comma 2 16" xfId="2937" xr:uid="{00000000-0005-0000-0000-0000130E0000}"/>
+    <cellStyle name="Comma 2 16 2" xfId="5501" xr:uid="{C8259521-70BA-463E-A2F8-AAB4235A12AF}"/>
     <cellStyle name="Comma 2 17" xfId="2933" xr:uid="{00000000-0005-0000-0000-0000140E0000}"/>
+    <cellStyle name="Comma 2 17 2" xfId="5500" xr:uid="{872D406F-7230-4F7A-A96A-230EAEC7B518}"/>
     <cellStyle name="Comma 2 18" xfId="2928" xr:uid="{00000000-0005-0000-0000-0000150E0000}"/>
+    <cellStyle name="Comma 2 18 2" xfId="5499" xr:uid="{53E54ACF-9C38-419C-BE21-E753B3249147}"/>
     <cellStyle name="Comma 2 19" xfId="2924" xr:uid="{00000000-0005-0000-0000-0000160E0000}"/>
+    <cellStyle name="Comma 2 19 2" xfId="5498" xr:uid="{71EAE5DF-0AB8-44B7-A939-1522A92A34F4}"/>
     <cellStyle name="Comma 2 2" xfId="3581" xr:uid="{00000000-0005-0000-0000-0000170E0000}"/>
     <cellStyle name="Comma 2 2 2" xfId="3580" xr:uid="{00000000-0005-0000-0000-0000180E0000}"/>
+    <cellStyle name="Comma 2 2 2 2" xfId="5524" xr:uid="{430921E2-ACD9-49F7-A4E0-94C2AA43EBA6}"/>
+    <cellStyle name="Comma 2 2 3" xfId="5525" xr:uid="{9734E46E-A9D8-419E-8A12-7893AC4ABB7C}"/>
     <cellStyle name="Comma 2 20" xfId="2921" xr:uid="{00000000-0005-0000-0000-0000190E0000}"/>
+    <cellStyle name="Comma 2 20 2" xfId="5497" xr:uid="{AA4E18D2-C484-4020-803A-E116BDC9CB79}"/>
     <cellStyle name="Comma 2 21" xfId="2917" xr:uid="{00000000-0005-0000-0000-00001A0E0000}"/>
+    <cellStyle name="Comma 2 21 2" xfId="5496" xr:uid="{37072A05-44AC-45A2-8897-582AB96F8300}"/>
     <cellStyle name="Comma 2 22" xfId="2913" xr:uid="{00000000-0005-0000-0000-00001B0E0000}"/>
+    <cellStyle name="Comma 2 22 2" xfId="5495" xr:uid="{B8B4B452-D314-48A4-8E6F-D92D5B137E00}"/>
     <cellStyle name="Comma 2 23" xfId="2910" xr:uid="{00000000-0005-0000-0000-00001C0E0000}"/>
+    <cellStyle name="Comma 2 23 2" xfId="5494" xr:uid="{E04071DD-68D4-42D7-9D25-1AD74D4A7BF0}"/>
     <cellStyle name="Comma 2 24" xfId="2907" xr:uid="{00000000-0005-0000-0000-00001D0E0000}"/>
+    <cellStyle name="Comma 2 24 2" xfId="5493" xr:uid="{E3CF2093-9488-4475-82C9-705459A82D92}"/>
     <cellStyle name="Comma 2 25" xfId="2904" xr:uid="{00000000-0005-0000-0000-00001E0E0000}"/>
+    <cellStyle name="Comma 2 25 2" xfId="5492" xr:uid="{92094969-29A8-4B1F-971A-D93EF13A632F}"/>
     <cellStyle name="Comma 2 26" xfId="2901" xr:uid="{00000000-0005-0000-0000-00001F0E0000}"/>
+    <cellStyle name="Comma 2 26 2" xfId="5491" xr:uid="{EEAC5A48-299B-4425-9236-158D1C2A79A5}"/>
     <cellStyle name="Comma 2 27" xfId="2898" xr:uid="{00000000-0005-0000-0000-0000200E0000}"/>
+    <cellStyle name="Comma 2 27 2" xfId="5490" xr:uid="{AD2C3EB1-D1AC-4185-BCB2-14EA40C2921A}"/>
     <cellStyle name="Comma 2 28" xfId="2894" xr:uid="{00000000-0005-0000-0000-0000210E0000}"/>
+    <cellStyle name="Comma 2 28 2" xfId="5489" xr:uid="{04796359-3ACC-4551-8A69-3D86F999D73A}"/>
     <cellStyle name="Comma 2 29" xfId="2889" xr:uid="{00000000-0005-0000-0000-0000220E0000}"/>
+    <cellStyle name="Comma 2 29 2" xfId="5488" xr:uid="{C614CF91-02F7-449E-AA77-1C4012CBBE56}"/>
     <cellStyle name="Comma 2 3" xfId="3579" xr:uid="{00000000-0005-0000-0000-0000230E0000}"/>
+    <cellStyle name="Comma 2 3 2" xfId="5523" xr:uid="{0011EAFE-70F9-41B7-B765-294BEF550699}"/>
     <cellStyle name="Comma 2 30" xfId="2883" xr:uid="{00000000-0005-0000-0000-0000240E0000}"/>
+    <cellStyle name="Comma 2 30 2" xfId="5487" xr:uid="{FD982C83-44BF-4DBE-99B3-98D441B58BB5}"/>
     <cellStyle name="Comma 2 31" xfId="2857" xr:uid="{00000000-0005-0000-0000-0000250E0000}"/>
+    <cellStyle name="Comma 2 31 2" xfId="5486" xr:uid="{1C78CDFE-F310-4C90-AF05-C98245DC9612}"/>
     <cellStyle name="Comma 2 32" xfId="2718" xr:uid="{00000000-0005-0000-0000-0000260E0000}"/>
+    <cellStyle name="Comma 2 32 2" xfId="5485" xr:uid="{2DA61F08-91CD-4B44-8382-0035D334630B}"/>
     <cellStyle name="Comma 2 33" xfId="2677" xr:uid="{00000000-0005-0000-0000-0000270E0000}"/>
+    <cellStyle name="Comma 2 33 2" xfId="5484" xr:uid="{F6E5D9F5-8871-40C5-87BF-95BE1C7F9B7E}"/>
     <cellStyle name="Comma 2 34" xfId="2641" xr:uid="{00000000-0005-0000-0000-0000280E0000}"/>
+    <cellStyle name="Comma 2 34 2" xfId="5483" xr:uid="{2B47EBDC-8F45-4A41-972E-38FA2BCDB186}"/>
+    <cellStyle name="Comma 2 35" xfId="5526" xr:uid="{1CFFA67D-36D7-4DE4-8D5D-288A25AAB6A0}"/>
     <cellStyle name="Comma 2 4" xfId="3578" xr:uid="{00000000-0005-0000-0000-0000290E0000}"/>
+    <cellStyle name="Comma 2 4 2" xfId="5522" xr:uid="{5E696856-F058-46A3-BBDB-CEC9917CD751}"/>
     <cellStyle name="Comma 2 5" xfId="3577" xr:uid="{00000000-0005-0000-0000-00002A0E0000}"/>
+    <cellStyle name="Comma 2 5 2" xfId="5521" xr:uid="{2633086A-C00D-4DC6-BF6B-2B4FD1DB5CAD}"/>
     <cellStyle name="Comma 2 6" xfId="3576" xr:uid="{00000000-0005-0000-0000-00002B0E0000}"/>
     <cellStyle name="Comma 2 6 2" xfId="2977" xr:uid="{00000000-0005-0000-0000-00002C0E0000}"/>
+    <cellStyle name="Comma 2 6 2 2" xfId="5510" xr:uid="{63019FAC-E184-4C8A-BA9A-DC96D4A4FDE1}"/>
+    <cellStyle name="Comma 2 6 3" xfId="5520" xr:uid="{D7B5404F-8766-4BFB-BF33-71866F263D7C}"/>
     <cellStyle name="Comma 2 7" xfId="3575" xr:uid="{00000000-0005-0000-0000-00002D0E0000}"/>
+    <cellStyle name="Comma 2 7 2" xfId="5519" xr:uid="{BFAF58B3-0F30-491C-A070-E4F54DFD8699}"/>
     <cellStyle name="Comma 2 8" xfId="2972" xr:uid="{00000000-0005-0000-0000-00002E0E0000}"/>
+    <cellStyle name="Comma 2 8 2" xfId="5509" xr:uid="{130013B2-FF94-4088-9C3E-17161066A3B3}"/>
     <cellStyle name="Comma 2 9" xfId="2969" xr:uid="{00000000-0005-0000-0000-00002F0E0000}"/>
+    <cellStyle name="Comma 2 9 2" xfId="5508" xr:uid="{50A6378B-77BF-4589-9A12-12947F22FF4F}"/>
     <cellStyle name="Comma 3" xfId="3574" xr:uid="{00000000-0005-0000-0000-0000300E0000}"/>
     <cellStyle name="Comma 3 2" xfId="2599" xr:uid="{00000000-0005-0000-0000-0000310E0000}"/>
+    <cellStyle name="Comma 3 2 2" xfId="5482" xr:uid="{9975A336-B286-4025-9C20-1FA70C2C99BA}"/>
     <cellStyle name="Comma 3 3" xfId="2598" xr:uid="{00000000-0005-0000-0000-0000320E0000}"/>
+    <cellStyle name="Comma 3 3 2" xfId="5481" xr:uid="{6EA02A7E-77A8-4872-8C26-36857FD2A183}"/>
     <cellStyle name="Comma 3 4" xfId="2597" xr:uid="{00000000-0005-0000-0000-0000330E0000}"/>
+    <cellStyle name="Comma 3 4 2" xfId="5480" xr:uid="{107B31A7-246D-4877-8321-CCA5D831B7CD}"/>
+    <cellStyle name="Comma 3 5" xfId="5518" xr:uid="{EE54E8B3-CFFC-468F-B362-938522CBCED3}"/>
     <cellStyle name="Comma 4" xfId="3573" xr:uid="{00000000-0005-0000-0000-0000340E0000}"/>
+    <cellStyle name="Comma 4 2" xfId="5517" xr:uid="{7FF9C336-6E5B-4AC0-9D12-047B946A8277}"/>
     <cellStyle name="Comma 5" xfId="3572" xr:uid="{00000000-0005-0000-0000-0000350E0000}"/>
     <cellStyle name="Comma 5 2" xfId="3571" xr:uid="{00000000-0005-0000-0000-0000360E0000}"/>
+    <cellStyle name="Comma 5 2 2" xfId="5515" xr:uid="{FF047124-EBB6-4279-A599-651F84E8BCAA}"/>
+    <cellStyle name="Comma 5 3" xfId="5516" xr:uid="{AA630B49-49D8-41E1-B452-CFDC8280E87F}"/>
     <cellStyle name="Comma 6" xfId="3570" xr:uid="{00000000-0005-0000-0000-0000370E0000}"/>
+    <cellStyle name="Comma 6 2" xfId="5514" xr:uid="{E0CECCB2-483A-44AE-8294-3AEAFB48573F}"/>
     <cellStyle name="Comma 7" xfId="3569" xr:uid="{00000000-0005-0000-0000-0000380E0000}"/>
+    <cellStyle name="Comma 7 2" xfId="5513" xr:uid="{EC8838E1-EC66-4E47-BAFB-4DDC06F35906}"/>
     <cellStyle name="Comma 8" xfId="3568" xr:uid="{00000000-0005-0000-0000-0000390E0000}"/>
+    <cellStyle name="Comma 8 2" xfId="5512" xr:uid="{6C0B086D-800D-4FB4-9F58-F70850906B49}"/>
     <cellStyle name="Comma 9" xfId="3567" xr:uid="{00000000-0005-0000-0000-00003A0E0000}"/>
+    <cellStyle name="Comma 9 2" xfId="5511" xr:uid="{5C025DFF-2323-4587-A13D-78C84AC4584B}"/>
     <cellStyle name="Currency 10" xfId="3566" xr:uid="{00000000-0005-0000-0000-00003B0E0000}"/>
     <cellStyle name="Currency 11" xfId="3565" xr:uid="{00000000-0005-0000-0000-00003C0E0000}"/>
     <cellStyle name="Currency 12" xfId="3564" xr:uid="{00000000-0005-0000-0000-00003D0E0000}"/>
@@ -12707,22 +12789,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV6"/>
+  <dimension ref="A1:AX6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="12" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="6" width="12.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="6" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="6" width="16.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="6" width="14.140625" collapsed="true"/>
+    <col min="1" max="1" style="9" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="12.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="14.140625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="7.5703125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="18.42578125" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="11" max="11" customWidth="true" width="8.7109375" collapsed="true"/>
@@ -12747,814 +12829,817 @@
     <col min="32" max="32" customWidth="true" width="18.85546875" collapsed="true"/>
     <col min="33" max="34" customWidth="true" width="21.7109375" collapsed="true"/>
     <col min="35" max="35" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="6" width="19.5703125" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="6" width="15.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="4" width="21.0" collapsed="true"/>
     <col min="38" max="38" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
-    <col min="39" max="16384" style="6" width="9.140625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" style="4" width="14.85546875" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" style="4" width="13.140625" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="4" width="17.85546875" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" style="4" width="14.85546875" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" style="4" width="15.85546875" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" style="4" width="21.7109375" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" style="4" width="17.140625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="4" width="21.5703125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="4" width="19.140625" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="4" width="17.85546875" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" style="4" width="21.0" collapsed="true"/>
+    <col min="50" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:49">
+      <c r="A1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH1" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AJ1" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AK1" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="AJ1" s="25" t="s">
+      <c r="AL1" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="AK1" s="25" t="s">
+      <c r="AM1" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="AL1" s="25" t="s">
+      <c r="AN1" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="AM1" s="25" t="s">
+      <c r="AO1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="AN1" s="25" t="s">
+      <c r="AP1" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" s="25" t="s">
+      <c r="AQ1" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="AP1" s="25" t="s">
+      <c r="AR1" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="AS1" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="AR1" s="25" t="s">
+      <c r="AT1" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="AS1" s="25" t="s">
+      <c r="AU1" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="AT1" s="25" t="s">
+      <c r="AV1" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="AU1" s="25" t="s">
+      <c r="AW1" s="38" t="s">
         <v>86</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="2" spans="1:47">
-      <c r="A2" s="13">
+    <row customHeight="1" ht="24" r="2" spans="1:49">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="13">
+      <c r="I2" s="7"/>
+      <c r="J2" s="10">
         <v>1</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="10">
         <v>0</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="T2" s="10">
+      <c r="T2" s="8">
         <v>45000</v>
       </c>
-      <c r="U2" s="10">
+      <c r="U2" s="8">
         <f>T2/4</f>
         <v>11250</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="V2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="W2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="X2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="Y2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10" t="s">
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="10" t="s">
+      <c r="AB2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AC2" s="10" t="s">
+      <c r="AC2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AD2" s="10" t="s">
+      <c r="AD2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AE2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AF2" s="10">
+      <c r="AF2" s="8">
         <v>1</v>
       </c>
-      <c r="AG2" s="10" t="s">
+      <c r="AG2" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH2" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI2" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="AH2" s="10" t="s">
+      <c r="AJ2" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="AI2" s="10" t="s">
+      <c r="AK2" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="AJ2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK2" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM2" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN2" s="15" t="s">
+      <c r="AL2" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM2" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN2" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO2" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP2" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="AO2" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="AP2" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="15"/>
-      <c r="AS2" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15" t="s">
-        <v>148</v>
-      </c>
+      <c r="AQ2" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR2" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="AS2" s="42"/>
+      <c r="AT2" s="42"/>
+      <c r="AU2" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="AV2" s="42"/>
+      <c r="AW2" s="42"/>
     </row>
-    <row customHeight="1" ht="24" r="3" spans="1:47">
-      <c r="A3" s="13">
+    <row customHeight="1" ht="24" r="3" spans="1:49">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="13">
+      <c r="I3" s="7"/>
+      <c r="J3" s="10">
         <v>1</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="10">
         <v>0</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="T3" s="10">
+      <c r="T3" s="8">
         <v>45000</v>
       </c>
-      <c r="U3" s="10">
+      <c r="U3" s="8">
         <f>T3/4</f>
         <v>11250</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="V3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="X3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="Y3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10" t="s">
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AB3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="AC3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AD3" s="10" t="s">
+      <c r="AD3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AE3" s="14" t="s">
+      <c r="AE3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="AF3" s="10">
+      <c r="AF3" s="8">
         <v>1</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AG3" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH3" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="AI3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AH3" s="10" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AI3" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK3" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="AM3" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="AN3" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="AO3" s="15"/>
-      <c r="AP3" s="15"/>
-      <c r="AQ3" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="AR3" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="AS3" s="15"/>
-      <c r="AT3" s="15"/>
-      <c r="AU3" s="15"/>
+      <c r="AK3" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL3" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM3" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN3" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO3" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP3" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="AQ3" s="42"/>
+      <c r="AR3" s="42"/>
+      <c r="AS3" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="AT3" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="AU3" s="42"/>
+      <c r="AV3" s="42"/>
+      <c r="AW3" s="42"/>
     </row>
-    <row customHeight="1" ht="24" r="4" spans="1:47">
-      <c r="A4" s="13">
+    <row customHeight="1" ht="24" r="4" spans="1:49">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="13">
+      <c r="I4" s="7"/>
+      <c r="J4" s="10">
         <v>1</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="10">
         <v>0</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="Q4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="R4" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="16" t="s">
+      <c r="S4" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4" s="8">
         <v>45000</v>
       </c>
-      <c r="U4" s="10">
+      <c r="U4" s="8">
         <f>T4/4</f>
         <v>11250</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="V4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="X4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Y4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10" t="s">
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AB4" s="10" t="s">
+      <c r="AB4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AC4" s="10" t="s">
+      <c r="AC4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AD4" s="10" t="s">
+      <c r="AD4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="15" t="s">
+      <c r="AE4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AF4" s="10">
+      <c r="AF4" s="8">
         <v>1</v>
       </c>
-      <c r="AG4" s="10" t="s">
+      <c r="AG4" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH4" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI4" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="AH4" s="10" t="s">
+      <c r="AJ4" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="AI4" s="10" t="s">
+      <c r="AK4" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="AJ4" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK4" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM4" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AN4" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="AO4" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP4" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AQ4" s="15"/>
-      <c r="AR4" s="15"/>
-      <c r="AS4" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="AT4" s="15"/>
-      <c r="AU4" s="15"/>
+      <c r="AL4" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM4" s="42"/>
+      <c r="AN4" s="42"/>
+      <c r="AO4" s="42"/>
+      <c r="AP4" s="42"/>
+      <c r="AQ4" s="42"/>
+      <c r="AR4" s="42"/>
+      <c r="AS4" s="42"/>
+      <c r="AT4" s="42"/>
+      <c r="AU4" s="42"/>
+      <c r="AV4" s="42"/>
+      <c r="AW4" s="42"/>
     </row>
-    <row customHeight="1" ht="24" r="5" spans="1:47">
-      <c r="A5" s="13">
+    <row customHeight="1" ht="24" r="5" spans="1:49">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="13">
+      <c r="I5" s="7"/>
+      <c r="J5" s="10">
         <v>1</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="10">
         <v>0</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R5" s="16" t="s">
+      <c r="R5" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="S5" s="16" t="s">
+      <c r="S5" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="T5" s="10">
+      <c r="T5" s="8">
         <v>45000</v>
       </c>
-      <c r="U5" s="10">
+      <c r="U5" s="8">
         <f>T5/4</f>
         <v>11250</v>
       </c>
-      <c r="V5" s="10" t="s">
+      <c r="V5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W5" s="10" t="s">
+      <c r="W5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="X5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="Y5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10" t="s">
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AB5" s="10" t="s">
+      <c r="AB5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AC5" s="10" t="s">
+      <c r="AC5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AD5" s="10" t="s">
+      <c r="AD5" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AE5" s="15" t="s">
+      <c r="AE5" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AF5" s="10">
+      <c r="AF5" s="8">
         <v>1</v>
       </c>
-      <c r="AG5" s="10" t="s">
+      <c r="AG5" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH5" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="AI5" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="AH5" s="10" t="s">
+      <c r="AJ5" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="AI5" s="10" t="s">
+      <c r="AK5" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="AJ5" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK5" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM5" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="AN5" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="AO5" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP5" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AQ5" s="15"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="15"/>
+      <c r="AL5" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM5" s="42"/>
+      <c r="AN5" s="42"/>
+      <c r="AO5" s="42"/>
+      <c r="AP5" s="42"/>
+      <c r="AQ5" s="42"/>
+      <c r="AR5" s="42"/>
+      <c r="AS5" s="42"/>
+      <c r="AT5" s="42"/>
+      <c r="AU5" s="42"/>
+      <c r="AV5" s="42"/>
+      <c r="AW5" s="42"/>
     </row>
-    <row customHeight="1" ht="24" r="6" spans="1:47">
-      <c r="A6" s="13">
+    <row customHeight="1" ht="24" r="6" spans="1:49">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="13">
+      <c r="I6" s="7"/>
+      <c r="J6" s="10">
         <v>1</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="10">
         <v>0</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="16" t="s">
+      <c r="R6" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="S6" s="16" t="s">
+      <c r="S6" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="T6" s="10">
+      <c r="T6" s="8">
         <v>45000</v>
       </c>
-      <c r="U6" s="10">
+      <c r="U6" s="8">
         <f>T6/4</f>
         <v>11250</v>
       </c>
-      <c r="V6" s="10" t="s">
+      <c r="V6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W6" s="10" t="s">
+      <c r="W6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="X6" s="10" t="s">
+      <c r="X6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="10" t="s">
+      <c r="Y6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10" t="s">
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AB6" s="10" t="s">
+      <c r="AB6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AC6" s="10" t="s">
+      <c r="AC6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AD6" s="10" t="s">
+      <c r="AD6" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AE6" s="15" t="s">
+      <c r="AE6" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AF6" s="10">
+      <c r="AF6" s="8">
         <v>1</v>
       </c>
-      <c r="AG6" s="10" t="s">
+      <c r="AG6" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH6" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH6" s="10" t="s">
+      <c r="AJ6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AI6" s="10" t="s">
+      <c r="AK6" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AJ6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK6" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="AL6" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM6" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="AN6" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO6" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="AP6" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="15"/>
+      <c r="AL6" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM6" s="42"/>
+      <c r="AN6" s="42"/>
+      <c r="AO6" s="42"/>
+      <c r="AP6" s="42"/>
+      <c r="AQ6" s="42"/>
+      <c r="AR6" s="42"/>
+      <c r="AS6" s="42"/>
+      <c r="AT6" s="42"/>
+      <c r="AU6" s="42"/>
+      <c r="AV6" s="42"/>
+      <c r="AW6" s="42"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -13566,7 +13651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
@@ -13583,8 +13668,8 @@
     <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
     <col min="17" max="21" customWidth="true" width="16.28515625" collapsed="true"/>
     <col min="22" max="22" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="6" width="19.5703125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="6" width="15.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="4" width="15.0" collapsed="true"/>
     <col min="25" max="25" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
     <col min="26" max="26" customWidth="true" width="15.140625" collapsed="true"/>
     <col min="27" max="27" customWidth="true" width="15.28515625" collapsed="true"/>
@@ -13597,192 +13682,192 @@
     <col min="34" max="34" customWidth="true" width="21.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="12.75" r="1" s="29" spans="1:31">
-      <c r="A1" s="26" t="s">
+    <row customFormat="1" ht="12.75" r="1" s="25" spans="1:31">
+      <c r="A1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="X1" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC1" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE1" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row customFormat="1" ht="12.75" r="2" s="25" spans="1:31">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="31"/>
+      <c r="M2" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="W1" s="27" t="s">
+      <c r="N2" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="R2" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="X2" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y2" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z2" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB2" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC2" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="AA1" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB1" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC1" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE1" s="39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row customFormat="1" ht="12.75" r="2" s="29" spans="1:31">
-      <c r="A2" s="30">
-        <v>1</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="31" t="s">
+      <c r="AD2" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="AE2" s="34" t="s">
         <v>124</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="K2" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="L2" s="35"/>
-      <c r="M2" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="N2" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="O2" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="P2" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="R2" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="T2" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="V2" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="W2" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="X2" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y2" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z2" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA2" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB2" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC2" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="AD2" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE2" s="38" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -13808,58 +13893,58 @@
   </cols>
   <sheetData>
     <row customHeight="1" ht="33" r="1" spans="1:4">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row ht="30" r="2" spans="1:4">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="18" t="s">
         <v>92</v>
       </c>
     </row>
     <row customHeight="1" ht="46.5" r="3" spans="1:4">
-      <c r="A3" s="20">
+      <c r="A3" s="17">
         <v>91111</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="18" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="20">
+      <c r="A4" s="17">
         <v>91111</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="18" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GL and WC Straight through Flow and GL Referral Flow Committed.
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="152">
   <si>
     <t>Class Code</t>
   </si>
@@ -470,6 +470,24 @@
   </si>
   <si>
     <t>$100</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-132478970</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-320616213</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-088125533</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-827323650</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-730421662</t>
+  </si>
+  <si>
+    <t>FWAL0020299100</t>
   </si>
 </sst>
 </file>
@@ -13864,10 +13882,10 @@
         <v>122</v>
       </c>
       <c r="AD2" s="27" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="AE2" s="34" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Notes and Messages Functions
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\New folder\FCGA-Version2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{8F17B4BB-AF58-4C84-846A-88E45ED4E7FE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
+  <xr:revisionPtr documentId="13_ncr:1_{58E70501-F971-4BE4-A325-BF2D8A22B364}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
     <workbookView windowHeight="13140" windowWidth="24240" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="147">
   <si>
     <t>Class Code</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Anderson</t>
-  </si>
-  <si>
-    <t>$1,000,000/$1,000,000</t>
   </si>
   <si>
     <t>$500</t>
@@ -282,13 +279,7 @@
     <t>Fullpay</t>
   </si>
   <si>
-    <t>10pay</t>
-  </si>
-  <si>
     <t>Check</t>
-  </si>
-  <si>
-    <t>Premium Finance</t>
   </si>
   <si>
     <t>Policy No.</t>
@@ -313,139 +304,166 @@
     <t>Does the Applicant use any cranes, lifts or bucket trucks?</t>
   </si>
   <si>
+    <t>Does the applicant perform ANY out of state work?</t>
+  </si>
+  <si>
+    <t>Insured Name</t>
+  </si>
+  <si>
+    <t>Quote Date</t>
+  </si>
+  <si>
+    <t>County Code</t>
+  </si>
+  <si>
+    <t>FWCI Premium</t>
+  </si>
+  <si>
+    <t>FWCI MGA Policy Fee</t>
+  </si>
+  <si>
+    <t>CB Premium</t>
+  </si>
+  <si>
+    <t>CB MGA Policy Fee</t>
+  </si>
+  <si>
+    <t>FWCI Producer Fee</t>
+  </si>
+  <si>
+    <t>CB Producer Fee</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>AddressState</t>
+  </si>
+  <si>
+    <t>PT_Gross Annual Payroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Officers Gross Annual Payroll</t>
+  </si>
+  <si>
+    <t>ContactEmail</t>
+  </si>
+  <si>
+    <t>ContactPhone</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Siddharth</t>
+  </si>
+  <si>
+    <t>187200</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>FWAL0020283000</t>
+  </si>
+  <si>
+    <t>Additional Insured</t>
+  </si>
+  <si>
+    <t>Raja Kumar</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-971427269</t>
+  </si>
+  <si>
+    <t>IRPM</t>
+  </si>
+  <si>
+    <t>Modified Rates</t>
+  </si>
+  <si>
+    <t>CTR</t>
+  </si>
+  <si>
+    <t>UW Rate Type</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
     <t>Does applicant  perform any roofing, roof work, or any activity of any kind on any roof, including any construction, repair, maintenance, cleaning or inspection of any roof?</t>
   </si>
   <si>
-    <t>Does the applicant perform ANY out of state work?</t>
+    <t>PremiumFinance</t>
+  </si>
+  <si>
+    <t>Referral Flow</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>Does applicant perform any roofing, roof work, or any activity of any kind on any roof, including any construction, repair, maintenance, cleaning or inspection of any roof?</t>
   </si>
   <si>
-    <t>Insured Name</t>
-  </si>
-  <si>
-    <t>Quote Date</t>
-  </si>
-  <si>
-    <t>County Code</t>
-  </si>
-  <si>
-    <t>FWCI Premium</t>
-  </si>
-  <si>
-    <t>FWCI MGA Policy Fee</t>
-  </si>
-  <si>
-    <t>CB Premium</t>
-  </si>
-  <si>
-    <t>CB MGA Policy Fee</t>
-  </si>
-  <si>
-    <t>FWCI Producer Fee</t>
-  </si>
-  <si>
-    <t>CB Producer Fee</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>4paybimonthly</t>
-  </si>
-  <si>
-    <t>4paymonthly</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>All Island Credit Corp.</t>
   </si>
   <si>
-    <t>AddressState</t>
-  </si>
-  <si>
-    <t>PT_Gross Annual Payroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Officers Gross Annual Payroll</t>
-  </si>
-  <si>
-    <t>ContactEmail</t>
-  </si>
-  <si>
-    <t>ContactPhone</t>
-  </si>
-  <si>
-    <t>Huntsville</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Address 1</t>
-  </si>
-  <si>
-    <t>35801</t>
-  </si>
-  <si>
-    <t>Siddharth</t>
-  </si>
-  <si>
-    <t>187200</t>
-  </si>
-  <si>
-    <t>test@test.com</t>
+    <t>$1,000,000/$1,000,000</t>
+  </si>
+  <si>
+    <t>10pay</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>FCGA AUTM -452371461</t>
+  </si>
+  <si>
+    <t>03/09/2020</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>$1,589</t>
+  </si>
+  <si>
+    <t>$90</t>
+  </si>
+  <si>
+    <t>$100</t>
+  </si>
+  <si>
+    <t>FGTX0020300000</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>FCGA AUTM-290247362</t>
-  </si>
-  <si>
-    <t>FWAL0020283000</t>
-  </si>
-  <si>
-    <t>Referral Flow</t>
-  </si>
-  <si>
-    <t>Additional Insured</t>
-  </si>
-  <si>
-    <t>Raja Kumar</t>
-  </si>
-  <si>
-    <t>UW Rate Type</t>
-  </si>
-  <si>
-    <t>Modified Rates</t>
-  </si>
-  <si>
-    <t>IRPM</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>CTR</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -020015449</t>
-  </si>
-  <si>
-    <t>03/09/2020</t>
-  </si>
-  <si>
-    <t/>
+    <t>FCGA AUTM -518075981</t>
+  </si>
+  <si>
+    <t>$2,749</t>
+  </si>
+  <si>
+    <t>FGTX0020300100</t>
+  </si>
+  <si>
+    <t>FCGA AUTM -836717690</t>
   </si>
   <si>
     <t>06</t>
@@ -455,39 +473,6 @@
   </si>
   <si>
     <t>$25</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -995180704</t>
-  </si>
-  <si>
-    <t>FCGA AUTM -771357723</t>
-  </si>
-  <si>
-    <t>$1,548</t>
-  </si>
-  <si>
-    <t>$90</t>
-  </si>
-  <si>
-    <t>$100</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-132478970</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-320616213</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-088125533</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-827323650</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-730421662</t>
-  </si>
-  <si>
-    <t>FWAL0020299100</t>
   </si>
 </sst>
 </file>
@@ -496,8 +481,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0;[Red]0"/>
     <numFmt numFmtId="167" formatCode="0000"/>
   </numFmts>
@@ -3657,42 +3642,42 @@
     <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="36" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="30" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
@@ -3836,13 +3821,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49">
       <alignment horizontal="right"/>
     </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="33" numFmtId="0">
       <alignment vertical="top"/>
@@ -3887,13 +3872,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
@@ -3925,19 +3910,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
@@ -3961,27 +3946,27 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
@@ -4005,14 +3990,14 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
@@ -4025,7 +4010,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
@@ -4035,10 +4020,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="9"/>
@@ -4056,46 +4041,46 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49">
       <alignment horizontal="right"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="9"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
@@ -4118,12 +4103,12 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49">
       <alignment horizontal="right"/>
     </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
@@ -4144,106 +4129,106 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
@@ -4296,14 +4281,14 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="9"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="32" numFmtId="0"/>
@@ -4807,68 +4792,68 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="30" numFmtId="2"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
@@ -4917,7 +4902,7 @@
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="29" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
@@ -6717,18 +6702,18 @@
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="7" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="7" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="34" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="165"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="35" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6782,7 +6767,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="36" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="37" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="165"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
@@ -6832,13 +6817,17 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -6853,6 +6842,9 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="2" numFmtId="166" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -6886,6 +6878,9 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="5">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="39" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="40" numFmtId="166" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -6925,23 +6920,38 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="39" fontId="40" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="2" numFmtId="49" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="37" fontId="2" numFmtId="166" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="39" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5528">
     <cellStyle name="20% - Accent1 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -10540,101 +10550,101 @@
     <cellStyle name="Check Cell 3 9" xfId="954" xr:uid="{00000000-0005-0000-0000-0000090E0000}"/>
     <cellStyle name="ColumnHeaderStyle" xfId="3008" xr:uid="{00000000-0005-0000-0000-00000A0E0000}"/>
     <cellStyle builtinId="3" name="Comma" xfId="5479"/>
-    <cellStyle name="Comma 10" xfId="5527" xr:uid="{2DB90E8E-B40C-4B4B-9530-BD8234A70FD7}"/>
+    <cellStyle name="Comma 10" xfId="5527" xr:uid="{219676D8-FD12-48D6-B1E2-ED2EF2CF1628}"/>
     <cellStyle name="Comma 2" xfId="3582" xr:uid="{00000000-0005-0000-0000-00000C0E0000}"/>
     <cellStyle name="Comma 2 10" xfId="2965" xr:uid="{00000000-0005-0000-0000-00000D0E0000}"/>
-    <cellStyle name="Comma 2 10 2" xfId="5507" xr:uid="{36CA78E7-1B40-4684-BD15-76F58D6BF49E}"/>
+    <cellStyle name="Comma 2 10 2" xfId="5507" xr:uid="{C2A5ECB9-8CF4-4B42-87B9-1D78133B5A22}"/>
     <cellStyle name="Comma 2 11" xfId="2961" xr:uid="{00000000-0005-0000-0000-00000E0E0000}"/>
-    <cellStyle name="Comma 2 11 2" xfId="5506" xr:uid="{0ED2D251-FAAB-4561-9702-67630FB654E1}"/>
+    <cellStyle name="Comma 2 11 2" xfId="5506" xr:uid="{0E3F339C-EC89-4E05-A86D-BEC6B9BDC76B}"/>
     <cellStyle name="Comma 2 12" xfId="2957" xr:uid="{00000000-0005-0000-0000-00000F0E0000}"/>
-    <cellStyle name="Comma 2 12 2" xfId="5505" xr:uid="{CE3718A9-5E91-490A-AE45-6F2F27C94CDA}"/>
+    <cellStyle name="Comma 2 12 2" xfId="5505" xr:uid="{08B1DA0B-8C3E-4EFF-AB14-DBF7CB6C2C64}"/>
     <cellStyle name="Comma 2 13" xfId="2953" xr:uid="{00000000-0005-0000-0000-0000100E0000}"/>
-    <cellStyle name="Comma 2 13 2" xfId="5504" xr:uid="{8DE2CED4-6BC4-43F9-AF01-55BF8CD4E5CC}"/>
+    <cellStyle name="Comma 2 13 2" xfId="5504" xr:uid="{B4B15423-B30E-407D-A24B-7ADF7B744178}"/>
     <cellStyle name="Comma 2 14" xfId="2948" xr:uid="{00000000-0005-0000-0000-0000110E0000}"/>
-    <cellStyle name="Comma 2 14 2" xfId="5503" xr:uid="{9DC33D54-1E4B-42FD-9647-854F85777C06}"/>
+    <cellStyle name="Comma 2 14 2" xfId="5503" xr:uid="{3E370192-0BBE-45FD-9CB3-C263345FA4CE}"/>
     <cellStyle name="Comma 2 15" xfId="2943" xr:uid="{00000000-0005-0000-0000-0000120E0000}"/>
-    <cellStyle name="Comma 2 15 2" xfId="5502" xr:uid="{581E18C0-40AC-4AA4-B9CE-5E09AD984DDA}"/>
+    <cellStyle name="Comma 2 15 2" xfId="5502" xr:uid="{D6B7A3F7-59D2-4DEB-A353-A7E52FF9E3CC}"/>
     <cellStyle name="Comma 2 16" xfId="2937" xr:uid="{00000000-0005-0000-0000-0000130E0000}"/>
-    <cellStyle name="Comma 2 16 2" xfId="5501" xr:uid="{C8259521-70BA-463E-A2F8-AAB4235A12AF}"/>
+    <cellStyle name="Comma 2 16 2" xfId="5501" xr:uid="{5009FC5A-9180-4058-8762-979CED3911B5}"/>
     <cellStyle name="Comma 2 17" xfId="2933" xr:uid="{00000000-0005-0000-0000-0000140E0000}"/>
-    <cellStyle name="Comma 2 17 2" xfId="5500" xr:uid="{872D406F-7230-4F7A-A96A-230EAEC7B518}"/>
+    <cellStyle name="Comma 2 17 2" xfId="5500" xr:uid="{56B19ABD-4EEA-4AB7-8895-52C64FBAAC93}"/>
     <cellStyle name="Comma 2 18" xfId="2928" xr:uid="{00000000-0005-0000-0000-0000150E0000}"/>
-    <cellStyle name="Comma 2 18 2" xfId="5499" xr:uid="{53E54ACF-9C38-419C-BE21-E753B3249147}"/>
+    <cellStyle name="Comma 2 18 2" xfId="5499" xr:uid="{BBEC625D-33ED-4AF7-9A6C-4E3C61C16CF6}"/>
     <cellStyle name="Comma 2 19" xfId="2924" xr:uid="{00000000-0005-0000-0000-0000160E0000}"/>
-    <cellStyle name="Comma 2 19 2" xfId="5498" xr:uid="{71EAE5DF-0AB8-44B7-A939-1522A92A34F4}"/>
+    <cellStyle name="Comma 2 19 2" xfId="5498" xr:uid="{8C6CDBED-1972-4502-BE36-1AE5D74F9CEE}"/>
     <cellStyle name="Comma 2 2" xfId="3581" xr:uid="{00000000-0005-0000-0000-0000170E0000}"/>
     <cellStyle name="Comma 2 2 2" xfId="3580" xr:uid="{00000000-0005-0000-0000-0000180E0000}"/>
-    <cellStyle name="Comma 2 2 2 2" xfId="5524" xr:uid="{430921E2-ACD9-49F7-A4E0-94C2AA43EBA6}"/>
-    <cellStyle name="Comma 2 2 3" xfId="5525" xr:uid="{9734E46E-A9D8-419E-8A12-7893AC4ABB7C}"/>
+    <cellStyle name="Comma 2 2 2 2" xfId="5524" xr:uid="{0E99D9A9-E83E-4E56-BE67-536AE9FF9E6F}"/>
+    <cellStyle name="Comma 2 2 3" xfId="5525" xr:uid="{A9FABC61-2B3D-4C39-A260-91AEBC84AC16}"/>
     <cellStyle name="Comma 2 20" xfId="2921" xr:uid="{00000000-0005-0000-0000-0000190E0000}"/>
-    <cellStyle name="Comma 2 20 2" xfId="5497" xr:uid="{AA4E18D2-C484-4020-803A-E116BDC9CB79}"/>
+    <cellStyle name="Comma 2 20 2" xfId="5497" xr:uid="{DF38C452-97BD-48A7-B416-D806C3BA30CA}"/>
     <cellStyle name="Comma 2 21" xfId="2917" xr:uid="{00000000-0005-0000-0000-00001A0E0000}"/>
-    <cellStyle name="Comma 2 21 2" xfId="5496" xr:uid="{37072A05-44AC-45A2-8897-582AB96F8300}"/>
+    <cellStyle name="Comma 2 21 2" xfId="5496" xr:uid="{095D46DA-E362-4016-A2FD-359CC984F6A5}"/>
     <cellStyle name="Comma 2 22" xfId="2913" xr:uid="{00000000-0005-0000-0000-00001B0E0000}"/>
-    <cellStyle name="Comma 2 22 2" xfId="5495" xr:uid="{B8B4B452-D314-48A4-8E6F-D92D5B137E00}"/>
+    <cellStyle name="Comma 2 22 2" xfId="5495" xr:uid="{A8F854CF-2E63-4D8B-96D1-6E54DB9A98C0}"/>
     <cellStyle name="Comma 2 23" xfId="2910" xr:uid="{00000000-0005-0000-0000-00001C0E0000}"/>
-    <cellStyle name="Comma 2 23 2" xfId="5494" xr:uid="{E04071DD-68D4-42D7-9D25-1AD74D4A7BF0}"/>
+    <cellStyle name="Comma 2 23 2" xfId="5494" xr:uid="{00780961-0B2A-4A3E-BEC9-F48627E47569}"/>
     <cellStyle name="Comma 2 24" xfId="2907" xr:uid="{00000000-0005-0000-0000-00001D0E0000}"/>
-    <cellStyle name="Comma 2 24 2" xfId="5493" xr:uid="{E3CF2093-9488-4475-82C9-705459A82D92}"/>
+    <cellStyle name="Comma 2 24 2" xfId="5493" xr:uid="{C8181A9C-D01B-419E-A290-285942CCA54E}"/>
     <cellStyle name="Comma 2 25" xfId="2904" xr:uid="{00000000-0005-0000-0000-00001E0E0000}"/>
-    <cellStyle name="Comma 2 25 2" xfId="5492" xr:uid="{92094969-29A8-4B1F-971A-D93EF13A632F}"/>
+    <cellStyle name="Comma 2 25 2" xfId="5492" xr:uid="{978BD4F0-EB57-491C-8236-8917BB477417}"/>
     <cellStyle name="Comma 2 26" xfId="2901" xr:uid="{00000000-0005-0000-0000-00001F0E0000}"/>
-    <cellStyle name="Comma 2 26 2" xfId="5491" xr:uid="{EEAC5A48-299B-4425-9236-158D1C2A79A5}"/>
+    <cellStyle name="Comma 2 26 2" xfId="5491" xr:uid="{08F7E04F-2502-4D39-ADFC-29C2C48E30F6}"/>
     <cellStyle name="Comma 2 27" xfId="2898" xr:uid="{00000000-0005-0000-0000-0000200E0000}"/>
-    <cellStyle name="Comma 2 27 2" xfId="5490" xr:uid="{AD2C3EB1-D1AC-4185-BCB2-14EA40C2921A}"/>
+    <cellStyle name="Comma 2 27 2" xfId="5490" xr:uid="{5A501559-B81E-47F8-92D4-56A8917A2A6A}"/>
     <cellStyle name="Comma 2 28" xfId="2894" xr:uid="{00000000-0005-0000-0000-0000210E0000}"/>
-    <cellStyle name="Comma 2 28 2" xfId="5489" xr:uid="{04796359-3ACC-4551-8A69-3D86F999D73A}"/>
+    <cellStyle name="Comma 2 28 2" xfId="5489" xr:uid="{39B47F54-741A-4C24-A40A-DC151906DBC8}"/>
     <cellStyle name="Comma 2 29" xfId="2889" xr:uid="{00000000-0005-0000-0000-0000220E0000}"/>
-    <cellStyle name="Comma 2 29 2" xfId="5488" xr:uid="{C614CF91-02F7-449E-AA77-1C4012CBBE56}"/>
+    <cellStyle name="Comma 2 29 2" xfId="5488" xr:uid="{47BBD87A-80D4-4ADD-889E-3D1ECD2B49EA}"/>
     <cellStyle name="Comma 2 3" xfId="3579" xr:uid="{00000000-0005-0000-0000-0000230E0000}"/>
-    <cellStyle name="Comma 2 3 2" xfId="5523" xr:uid="{0011EAFE-70F9-41B7-B765-294BEF550699}"/>
+    <cellStyle name="Comma 2 3 2" xfId="5523" xr:uid="{2E5F336F-C35D-4C7B-A2AD-394703499B9C}"/>
     <cellStyle name="Comma 2 30" xfId="2883" xr:uid="{00000000-0005-0000-0000-0000240E0000}"/>
-    <cellStyle name="Comma 2 30 2" xfId="5487" xr:uid="{FD982C83-44BF-4DBE-99B3-98D441B58BB5}"/>
+    <cellStyle name="Comma 2 30 2" xfId="5487" xr:uid="{BB4B71BF-0FAC-46F3-9FD0-D488C4A024E2}"/>
     <cellStyle name="Comma 2 31" xfId="2857" xr:uid="{00000000-0005-0000-0000-0000250E0000}"/>
-    <cellStyle name="Comma 2 31 2" xfId="5486" xr:uid="{1C78CDFE-F310-4C90-AF05-C98245DC9612}"/>
+    <cellStyle name="Comma 2 31 2" xfId="5486" xr:uid="{BE4266CE-1E9D-418B-9061-7D04A57A6EFC}"/>
     <cellStyle name="Comma 2 32" xfId="2718" xr:uid="{00000000-0005-0000-0000-0000260E0000}"/>
-    <cellStyle name="Comma 2 32 2" xfId="5485" xr:uid="{2DA61F08-91CD-4B44-8382-0035D334630B}"/>
+    <cellStyle name="Comma 2 32 2" xfId="5485" xr:uid="{BFD5D31D-744A-4B39-B992-7B96E40108D2}"/>
     <cellStyle name="Comma 2 33" xfId="2677" xr:uid="{00000000-0005-0000-0000-0000270E0000}"/>
-    <cellStyle name="Comma 2 33 2" xfId="5484" xr:uid="{F6E5D9F5-8871-40C5-87BF-95BE1C7F9B7E}"/>
+    <cellStyle name="Comma 2 33 2" xfId="5484" xr:uid="{94D67A6B-8F5D-4B8B-BB02-B3AA1770E708}"/>
     <cellStyle name="Comma 2 34" xfId="2641" xr:uid="{00000000-0005-0000-0000-0000280E0000}"/>
-    <cellStyle name="Comma 2 34 2" xfId="5483" xr:uid="{2B47EBDC-8F45-4A41-972E-38FA2BCDB186}"/>
-    <cellStyle name="Comma 2 35" xfId="5526" xr:uid="{1CFFA67D-36D7-4DE4-8D5D-288A25AAB6A0}"/>
+    <cellStyle name="Comma 2 34 2" xfId="5483" xr:uid="{ECC7D68F-95C5-4C84-AEFF-60E62EE6DD89}"/>
+    <cellStyle name="Comma 2 35" xfId="5526" xr:uid="{E8696705-F5B0-4FC1-94B8-9C807B5CA7D0}"/>
     <cellStyle name="Comma 2 4" xfId="3578" xr:uid="{00000000-0005-0000-0000-0000290E0000}"/>
-    <cellStyle name="Comma 2 4 2" xfId="5522" xr:uid="{5E696856-F058-46A3-BBDB-CEC9917CD751}"/>
+    <cellStyle name="Comma 2 4 2" xfId="5522" xr:uid="{5009AB8A-F076-4009-9B72-638F7CEC2AA9}"/>
     <cellStyle name="Comma 2 5" xfId="3577" xr:uid="{00000000-0005-0000-0000-00002A0E0000}"/>
-    <cellStyle name="Comma 2 5 2" xfId="5521" xr:uid="{2633086A-C00D-4DC6-BF6B-2B4FD1DB5CAD}"/>
+    <cellStyle name="Comma 2 5 2" xfId="5521" xr:uid="{78A2964F-9BE1-40B5-9578-597581C43126}"/>
     <cellStyle name="Comma 2 6" xfId="3576" xr:uid="{00000000-0005-0000-0000-00002B0E0000}"/>
     <cellStyle name="Comma 2 6 2" xfId="2977" xr:uid="{00000000-0005-0000-0000-00002C0E0000}"/>
-    <cellStyle name="Comma 2 6 2 2" xfId="5510" xr:uid="{63019FAC-E184-4C8A-BA9A-DC96D4A4FDE1}"/>
-    <cellStyle name="Comma 2 6 3" xfId="5520" xr:uid="{D7B5404F-8766-4BFB-BF33-71866F263D7C}"/>
+    <cellStyle name="Comma 2 6 2 2" xfId="5510" xr:uid="{23681E7A-FE9B-4214-A03B-0743AA816FE7}"/>
+    <cellStyle name="Comma 2 6 3" xfId="5520" xr:uid="{7AD0FDAB-F3FA-4023-B9E2-36EC6166F428}"/>
     <cellStyle name="Comma 2 7" xfId="3575" xr:uid="{00000000-0005-0000-0000-00002D0E0000}"/>
-    <cellStyle name="Comma 2 7 2" xfId="5519" xr:uid="{BFAF58B3-0F30-491C-A070-E4F54DFD8699}"/>
+    <cellStyle name="Comma 2 7 2" xfId="5519" xr:uid="{E519C9C6-8D4C-43D7-81C5-53561DD182AA}"/>
     <cellStyle name="Comma 2 8" xfId="2972" xr:uid="{00000000-0005-0000-0000-00002E0E0000}"/>
-    <cellStyle name="Comma 2 8 2" xfId="5509" xr:uid="{130013B2-FF94-4088-9C3E-17161066A3B3}"/>
+    <cellStyle name="Comma 2 8 2" xfId="5509" xr:uid="{D59A87FB-EE9E-4808-8B8A-A4E0EB922989}"/>
     <cellStyle name="Comma 2 9" xfId="2969" xr:uid="{00000000-0005-0000-0000-00002F0E0000}"/>
-    <cellStyle name="Comma 2 9 2" xfId="5508" xr:uid="{50A6378B-77BF-4589-9A12-12947F22FF4F}"/>
+    <cellStyle name="Comma 2 9 2" xfId="5508" xr:uid="{7AAB1A0F-433B-48CE-BC63-BD543D50E702}"/>
     <cellStyle name="Comma 3" xfId="3574" xr:uid="{00000000-0005-0000-0000-0000300E0000}"/>
     <cellStyle name="Comma 3 2" xfId="2599" xr:uid="{00000000-0005-0000-0000-0000310E0000}"/>
-    <cellStyle name="Comma 3 2 2" xfId="5482" xr:uid="{9975A336-B286-4025-9C20-1FA70C2C99BA}"/>
+    <cellStyle name="Comma 3 2 2" xfId="5482" xr:uid="{64A7DF66-298F-448D-8A0C-72DF55CCC76F}"/>
     <cellStyle name="Comma 3 3" xfId="2598" xr:uid="{00000000-0005-0000-0000-0000320E0000}"/>
-    <cellStyle name="Comma 3 3 2" xfId="5481" xr:uid="{6EA02A7E-77A8-4872-8C26-36857FD2A183}"/>
+    <cellStyle name="Comma 3 3 2" xfId="5481" xr:uid="{4D067518-F592-4AA4-AC18-8C0C919A7B78}"/>
     <cellStyle name="Comma 3 4" xfId="2597" xr:uid="{00000000-0005-0000-0000-0000330E0000}"/>
-    <cellStyle name="Comma 3 4 2" xfId="5480" xr:uid="{107B31A7-246D-4877-8321-CCA5D831B7CD}"/>
-    <cellStyle name="Comma 3 5" xfId="5518" xr:uid="{EE54E8B3-CFFC-468F-B362-938522CBCED3}"/>
+    <cellStyle name="Comma 3 4 2" xfId="5480" xr:uid="{49B6A3AE-7322-44B1-A19E-20971319386B}"/>
+    <cellStyle name="Comma 3 5" xfId="5518" xr:uid="{CB0F4597-579E-4D2A-8973-756264ABF10D}"/>
     <cellStyle name="Comma 4" xfId="3573" xr:uid="{00000000-0005-0000-0000-0000340E0000}"/>
-    <cellStyle name="Comma 4 2" xfId="5517" xr:uid="{7FF9C336-6E5B-4AC0-9D12-047B946A8277}"/>
+    <cellStyle name="Comma 4 2" xfId="5517" xr:uid="{26DDC3A1-C5D6-4515-BC63-3B3014386C50}"/>
     <cellStyle name="Comma 5" xfId="3572" xr:uid="{00000000-0005-0000-0000-0000350E0000}"/>
     <cellStyle name="Comma 5 2" xfId="3571" xr:uid="{00000000-0005-0000-0000-0000360E0000}"/>
-    <cellStyle name="Comma 5 2 2" xfId="5515" xr:uid="{FF047124-EBB6-4279-A599-651F84E8BCAA}"/>
-    <cellStyle name="Comma 5 3" xfId="5516" xr:uid="{AA630B49-49D8-41E1-B452-CFDC8280E87F}"/>
+    <cellStyle name="Comma 5 2 2" xfId="5515" xr:uid="{B4A0BA76-A740-4A25-83A9-CA91D505F521}"/>
+    <cellStyle name="Comma 5 3" xfId="5516" xr:uid="{8839291C-1031-4AA0-9906-B49504BA4D36}"/>
     <cellStyle name="Comma 6" xfId="3570" xr:uid="{00000000-0005-0000-0000-0000370E0000}"/>
-    <cellStyle name="Comma 6 2" xfId="5514" xr:uid="{E0CECCB2-483A-44AE-8294-3AEAFB48573F}"/>
+    <cellStyle name="Comma 6 2" xfId="5514" xr:uid="{9D61FD10-D3EB-465B-A0E1-7D0EEBE5FA43}"/>
     <cellStyle name="Comma 7" xfId="3569" xr:uid="{00000000-0005-0000-0000-0000380E0000}"/>
-    <cellStyle name="Comma 7 2" xfId="5513" xr:uid="{EC8838E1-EC66-4E47-BAFB-4DDC06F35906}"/>
+    <cellStyle name="Comma 7 2" xfId="5513" xr:uid="{B1976DEF-CFC1-4077-BCE5-E7B96F20A156}"/>
     <cellStyle name="Comma 8" xfId="3568" xr:uid="{00000000-0005-0000-0000-0000390E0000}"/>
-    <cellStyle name="Comma 8 2" xfId="5512" xr:uid="{6C0B086D-800D-4FB4-9F58-F70850906B49}"/>
+    <cellStyle name="Comma 8 2" xfId="5512" xr:uid="{DC7A943A-F273-4238-A08B-DA851C80BF87}"/>
     <cellStyle name="Comma 9" xfId="3567" xr:uid="{00000000-0005-0000-0000-00003A0E0000}"/>
-    <cellStyle name="Comma 9 2" xfId="5511" xr:uid="{5C025DFF-2323-4587-A13D-78C84AC4584B}"/>
+    <cellStyle name="Comma 9 2" xfId="5511" xr:uid="{54FDC223-B2E9-4ACA-AC94-E37275C19119}"/>
     <cellStyle name="Currency 10" xfId="3566" xr:uid="{00000000-0005-0000-0000-00003B0E0000}"/>
     <cellStyle name="Currency 11" xfId="3565" xr:uid="{00000000-0005-0000-0000-00003C0E0000}"/>
     <cellStyle name="Currency 12" xfId="3564" xr:uid="{00000000-0005-0000-0000-00003D0E0000}"/>
@@ -12807,22 +12817,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX6"/>
+  <dimension ref="A1:AX4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="9" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="12.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="16.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.140625" collapsed="true"/>
+    <col min="1" max="1" style="12" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="12.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="6" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="6" width="14.140625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="7.5703125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="18.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="11" max="11" customWidth="true" width="8.7109375" collapsed="true"/>
@@ -12844,820 +12854,587 @@
     <col min="29" max="29" customWidth="true" width="17.140625" collapsed="true"/>
     <col min="30" max="30" customWidth="true" width="16.28515625" collapsed="true"/>
     <col min="31" max="31" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="33" max="34" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="4" width="21.0" collapsed="true"/>
-    <col min="38" max="38" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
-    <col min="39" max="39" customWidth="true" style="4" width="14.85546875" collapsed="true"/>
-    <col min="40" max="40" customWidth="true" style="4" width="13.140625" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" style="4" width="17.85546875" collapsed="true"/>
-    <col min="42" max="42" customWidth="true" style="4" width="14.85546875" collapsed="true"/>
-    <col min="43" max="43" customWidth="true" style="4" width="15.85546875" collapsed="true"/>
-    <col min="44" max="44" customWidth="true" style="4" width="21.7109375" collapsed="true"/>
-    <col min="45" max="45" customWidth="true" style="4" width="17.140625" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" style="4" width="21.5703125" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" style="4" width="19.140625" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" style="4" width="17.85546875" collapsed="true"/>
-    <col min="49" max="49" customWidth="true" style="4" width="21.0" collapsed="true"/>
-    <col min="50" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="32" max="34" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="35" max="36" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" style="6" width="14.0" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" style="6" width="21.42578125" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="6" width="12.0" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" style="6" width="13.28515625" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" style="6" width="14.28515625" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" style="6" width="20.7109375" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" style="6" width="15.28515625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="6" width="18.5703125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="6" width="19.42578125" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="6" width="15.85546875" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" style="6" width="14.28515625" collapsed="true"/>
+    <col min="50" max="16384" style="6" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="AA1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AC1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC1" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD1" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE1" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF1" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG1" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH1" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="AI1" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ1" s="36" t="s">
+      <c r="AK1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AK1" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL1" s="38" t="s">
+      <c r="AL1" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="38" t="s">
+      <c r="AM1" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN1" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP1" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ1" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR1" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS1" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="AN1" s="38" t="s">
+      <c r="AT1" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="AO1" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP1" s="38" t="s">
+      <c r="AU1" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="AQ1" s="38" t="s">
+      <c r="AV1" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="AR1" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS1" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT1" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="AU1" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="AV1" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="AW1" s="38" t="s">
-        <v>86</v>
+      <c r="AW1" s="25" t="s">
+        <v>83</v>
       </c>
     </row>
     <row customHeight="1" ht="24" r="2" spans="1:49">
-      <c r="A2" s="10">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="10">
+      <c r="H2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="13">
         <v>1</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="13">
         <v>0</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="T2" s="8">
+      <c r="R2" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="T2" s="10">
         <v>45000</v>
       </c>
-      <c r="U2" s="8">
+      <c r="U2" s="10">
         <f>T2/4</f>
         <v>11250</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="8" t="s">
+      <c r="V2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AC2" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AD2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AE2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="AE2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF2" s="8">
+      <c r="AF2" s="10">
         <v>1</v>
       </c>
-      <c r="AG2" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="AH2" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="AI2" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ2" s="39" t="s">
+      <c r="AG2" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH2" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AI2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK2" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AK2" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL2" s="40" t="s">
+      <c r="AL2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO2" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="AM2" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN2" s="42" t="s">
+      <c r="AP2" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ2" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="AR2" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="AO2" s="42" t="s">
+      <c r="AS2" s="15"/>
+      <c r="AT2" s="15"/>
+      <c r="AU2" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="AP2" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="AQ2" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="AR2" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="AS2" s="42"/>
-      <c r="AT2" s="42"/>
-      <c r="AU2" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="AV2" s="42"/>
-      <c r="AW2" s="42"/>
+      <c r="AV2" s="15"/>
+      <c r="AW2" s="15" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row customHeight="1" ht="24" r="3" spans="1:49">
-      <c r="A3" s="10">
+      <c r="A3" s="49">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="F3" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="47"/>
+      <c r="J3" s="49">
+        <v>1</v>
+      </c>
+      <c r="K3" s="49">
+        <v>0</v>
+      </c>
+      <c r="L3" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="N3" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="S3" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="T3" s="48">
+        <v>45000</v>
+      </c>
+      <c r="U3" s="48">
+        <v>11250</v>
+      </c>
+      <c r="V3" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="10">
+      <c r="W3" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE3" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF3" s="48">
         <v>1</v>
       </c>
-      <c r="K3" s="10">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="T3" s="8">
-        <v>45000</v>
-      </c>
-      <c r="U3" s="8">
-        <f>T3/4</f>
-        <v>11250</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF3" s="8">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="AH3" s="41" t="s">
+      <c r="AG3" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI3" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ3" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="AK3" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL3" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM3" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN3" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="AI3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AL3" s="40" t="s">
+      <c r="AO3" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="AM3" s="42" t="s">
+      <c r="AP3" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ3" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="AN3" s="42" t="s">
+      <c r="AR3" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="AO3" s="42" t="s">
+      <c r="AS3" s="50"/>
+      <c r="AT3" s="50"/>
+      <c r="AU3" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="AP3" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="AQ3" s="42"/>
-      <c r="AR3" s="42"/>
-      <c r="AS3" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="AT3" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="AU3" s="42"/>
-      <c r="AV3" s="42"/>
-      <c r="AW3" s="42"/>
+      <c r="AV3" s="15"/>
+      <c r="AW3" s="15" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row customHeight="1" ht="24" r="4" spans="1:49">
-      <c r="A4" s="10">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="10">
+      <c r="F4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="13">
         <v>1</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="13">
         <v>0</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="8" t="s">
+      <c r="M4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="T4" s="8">
+      <c r="R4" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="S4" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="T4" s="10">
         <v>45000</v>
       </c>
-      <c r="U4" s="8">
+      <c r="U4" s="10">
         <f>T4/4</f>
         <v>11250</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="V4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="W4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="X4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC4" s="8" t="s">
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AE4" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF4" s="8">
+      <c r="AF4" s="10">
         <v>1</v>
       </c>
-      <c r="AG4" s="41" t="s">
+      <c r="AG4" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="AH4" s="41" t="s">
+      <c r="AH4" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="AI4" s="39" t="s">
+      <c r="AI4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="AJ4" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="AK4" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL4" s="40" t="s">
+      <c r="AJ4" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK4" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN4" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO4" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="AM4" s="42"/>
-      <c r="AN4" s="42"/>
-      <c r="AO4" s="42"/>
-      <c r="AP4" s="42"/>
-      <c r="AQ4" s="42"/>
-      <c r="AR4" s="42"/>
-      <c r="AS4" s="42"/>
-      <c r="AT4" s="42"/>
-      <c r="AU4" s="42"/>
-      <c r="AV4" s="42"/>
-      <c r="AW4" s="42"/>
-    </row>
-    <row customHeight="1" ht="24" r="5" spans="1:49">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="10">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="T5" s="8">
-        <v>45000</v>
-      </c>
-      <c r="U5" s="8">
-        <f>T5/4</f>
-        <v>11250</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="W5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="X5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF5" s="8">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="AH5" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="AI5" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ5" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK5" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL5" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="AM5" s="42"/>
-      <c r="AN5" s="42"/>
-      <c r="AO5" s="42"/>
-      <c r="AP5" s="42"/>
-      <c r="AQ5" s="42"/>
-      <c r="AR5" s="42"/>
-      <c r="AS5" s="42"/>
-      <c r="AT5" s="42"/>
-      <c r="AU5" s="42"/>
-      <c r="AV5" s="42"/>
-      <c r="AW5" s="42"/>
-    </row>
-    <row customHeight="1" ht="24" r="6" spans="1:49">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="10">
-        <v>1</v>
-      </c>
-      <c r="K6" s="10">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="R6" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="T6" s="8">
-        <v>45000</v>
-      </c>
-      <c r="U6" s="8">
-        <f>T6/4</f>
-        <v>11250</v>
-      </c>
-      <c r="V6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="W6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="X6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF6" s="8">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="AH6" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="AI6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL6" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="AM6" s="42"/>
-      <c r="AN6" s="42"/>
-      <c r="AO6" s="42"/>
-      <c r="AP6" s="42"/>
-      <c r="AQ6" s="42"/>
-      <c r="AR6" s="42"/>
-      <c r="AS6" s="42"/>
-      <c r="AT6" s="42"/>
-      <c r="AU6" s="42"/>
-      <c r="AV6" s="42"/>
-      <c r="AW6" s="42"/>
+      <c r="AP4" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="AQ4" s="15"/>
+      <c r="AR4" s="15"/>
+      <c r="AS4" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="AT4" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU4" s="15"/>
+      <c r="AV4" s="15"/>
+      <c r="AW4" s="15"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -13670,7 +13447,7 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13686,8 +13463,8 @@
     <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
     <col min="17" max="21" customWidth="true" width="16.28515625" collapsed="true"/>
     <col min="22" max="22" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="6" width="19.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="6" width="15.0" collapsed="true"/>
     <col min="25" max="25" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
     <col min="26" max="26" customWidth="true" width="15.140625" collapsed="true"/>
     <col min="27" max="27" customWidth="true" width="15.28515625" collapsed="true"/>
@@ -13700,192 +13477,192 @@
     <col min="34" max="34" customWidth="true" width="21.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="12.75" r="1" s="25" spans="1:31">
-      <c r="A1" s="22" t="s">
+    <row customFormat="1" ht="12.75" r="1" s="29" spans="1:31">
+      <c r="A1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="23" t="s">
+      <c r="F1" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y1" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z1" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA1" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC1" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE1" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" ht="12.75" r="2" s="29" spans="1:31">
+      <c r="A2" s="30">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="R2" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="T2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="W2" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="X2" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y2" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="K1" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="W1" s="23" t="s">
+      <c r="Z2" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB2" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC2" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD2" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE2" s="38" t="s">
         <v>111</v>
-      </c>
-      <c r="X1" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y1" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z1" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA1" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB1" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC1" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE1" s="35" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row customFormat="1" ht="12.75" r="2" s="25" spans="1:31">
-      <c r="A2" s="26">
-        <v>1</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="O2" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="P2" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="R2" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="T2" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="X2" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y2" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z2" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA2" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB2" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC2" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="AD2" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE2" s="34" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -13898,8 +13675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13911,59 +13688,59 @@
   </cols>
   <sheetData>
     <row customHeight="1" ht="33" r="1" spans="1:4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>90</v>
+      <c r="B1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row ht="30" r="2" spans="1:4">
-      <c r="A2" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>92</v>
+      <c r="A2" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>89</v>
       </c>
     </row>
     <row customHeight="1" ht="46.5" r="3" spans="1:4">
-      <c r="A3" s="17">
+      <c r="A3" s="20">
         <v>91111</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>95</v>
+      <c r="B3" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="17">
+      <c r="A4" s="20">
         <v>91111</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>94</v>
+      <c r="B4" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Completion of GL Product both Agent and UW.
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="7575" windowWidth="19320" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="2" windowHeight="7455" windowWidth="19200" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TD_GL" r:id="rId1" sheetId="3"/>
@@ -32,15 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="268">
   <si>
     <t>Class Code</t>
   </si>
   <si>
     <t>Quote No.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experience </t>
   </si>
   <si>
     <t>Claims</t>
@@ -518,18 +515,6 @@
     <t>CAR</t>
   </si>
   <si>
-    <t>$90</t>
-  </si>
-  <si>
-    <t>$100</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>$25</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -638,18 +623,9 @@
     <t>Matched/ Not Matched (TC-03)</t>
   </si>
   <si>
-    <t>FGTX0020332000</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>BGFL0020332200</t>
-  </si>
-  <si>
     <t>UWModify Expected Gross</t>
   </si>
   <si>
@@ -674,9 +650,6 @@
     <t>34000</t>
   </si>
   <si>
-    <t>$1,235</t>
-  </si>
-  <si>
     <t>Andrews</t>
   </si>
   <si>
@@ -690,18 +663,6 @@
   </si>
   <si>
     <t>Declined</t>
-  </si>
-  <si>
-    <t>04/10/2020</t>
-  </si>
-  <si>
-    <t>$3,697</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-285899141</t>
-  </si>
-  <si>
-    <t>Q-44282</t>
   </si>
   <si>
     <t>Does the Applicant do any work involving storage, manufacturing, distributing or dispensing of LPG-liquid propane gas?</t>
@@ -729,28 +690,154 @@
     <t>Referral Class codes</t>
   </si>
   <si>
+    <t>UW Referral Reason</t>
+  </si>
+  <si>
+    <t>OK -- Approved for Referral</t>
+  </si>
+  <si>
+    <t>UWModify State</t>
+  </si>
+  <si>
+    <t>UWModify City</t>
+  </si>
+  <si>
+    <t>UWModify Zip</t>
+  </si>
+  <si>
+    <t>Inspector Name</t>
+  </si>
+  <si>
+    <t>Rahul Sharma</t>
+  </si>
+  <si>
+    <t>LicenseType</t>
+  </si>
+  <si>
+    <t>License No.</t>
+  </si>
+  <si>
+    <t>Industrial Percent</t>
+  </si>
+  <si>
+    <t>Commercial Percent</t>
+  </si>
+  <si>
+    <t>Residential Percent</t>
+  </si>
+  <si>
+    <t>New Construction Percent</t>
+  </si>
+  <si>
+    <t>Room Additions Percent</t>
+  </si>
+  <si>
+    <t>Remodeling Percent</t>
+  </si>
+  <si>
+    <t>RepairorService Percent</t>
+  </si>
+  <si>
+    <t>EW-5465464</t>
+  </si>
+  <si>
+    <t>QS-4346464</t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
+  <si>
+    <t>Temperary</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Addrress1</t>
+  </si>
+  <si>
+    <t>EW-866896</t>
+  </si>
+  <si>
     <t>Matched</t>
   </si>
   <si>
     <t>Not Matched</t>
   </si>
   <si>
-    <t>FCGA AUTM-996188648</t>
-  </si>
-  <si>
-    <t>Q-44283</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-777002245</t>
-  </si>
-  <si>
-    <t>Q-44285</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-024024844</t>
-  </si>
-  <si>
-    <t>Q-44288</t>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Producer Fee</t>
+  </si>
+  <si>
+    <t>Description Of Business</t>
+  </si>
+  <si>
+    <t>Years In Business</t>
+  </si>
+  <si>
+    <t>Years In Trade</t>
+  </si>
+  <si>
+    <t>Business Desc.</t>
+  </si>
+  <si>
+    <t>Sub Contractor Description</t>
+  </si>
+  <si>
+    <t>OK-Approved</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-212907442</t>
+  </si>
+  <si>
+    <t>04/13/2020</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>$4,091</t>
+  </si>
+  <si>
+    <t>$25</t>
+  </si>
+  <si>
+    <t>FGFL0020334300</t>
+  </si>
+  <si>
+    <t>Matched/ Not Matched (TC-04)</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-550105751</t>
+  </si>
+  <si>
+    <t>$3,922</t>
+  </si>
+  <si>
+    <t>$90</t>
+  </si>
+  <si>
+    <t>$100</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-172414120</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>$1,235</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-726550805</t>
   </si>
 </sst>
 </file>
@@ -13084,10 +13171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CU3"/>
+  <dimension ref="A1:DM5"/>
   <sheetViews>
-    <sheetView topLeftCell="CA1" workbookViewId="0">
-      <selection activeCell="CD9" sqref="CD9"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13102,911 +13189,1714 @@
     <col min="8" max="8" customWidth="true" style="2" width="18.42578125" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="23" max="24" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="24" width="27.85546875" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="27" max="28" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="24" width="20.28515625" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="24" width="31.0" collapsed="true"/>
-    <col min="31" max="44" customWidth="true" style="24" width="28.140625" collapsed="true"/>
-    <col min="45" max="45" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="49" max="51" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="52" max="52" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="53" max="53" customWidth="true" style="24" width="25.7109375" collapsed="true"/>
-    <col min="54" max="54" customWidth="true" style="24" width="25.140625" collapsed="true"/>
-    <col min="55" max="55" customWidth="true" style="24" width="29.0" collapsed="true"/>
-    <col min="56" max="56" customWidth="true" style="24" width="30.7109375" collapsed="true"/>
-    <col min="57" max="57" customWidth="true" style="24" width="25.7109375" collapsed="true"/>
-    <col min="58" max="58" customWidth="true" style="24" width="27.7109375" collapsed="true"/>
-    <col min="59" max="59" customWidth="true" style="24" width="24.0" collapsed="true"/>
-    <col min="60" max="62" customWidth="true" style="24" width="29.5703125" collapsed="true"/>
-    <col min="63" max="70" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
-    <col min="71" max="71" customWidth="true" style="24" width="26.28515625" collapsed="true"/>
-    <col min="72" max="73" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
-    <col min="74" max="77" customWidth="true" style="24" width="24.7109375" collapsed="true"/>
-    <col min="78" max="78" customWidth="true" style="24" width="30.5703125" collapsed="true"/>
-    <col min="79" max="79" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="80" max="80" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="81" max="83" customWidth="true" style="24" width="24.85546875" collapsed="true"/>
-    <col min="84" max="84" customWidth="true" style="2" width="14.0" collapsed="true"/>
-    <col min="85" max="85" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
-    <col min="86" max="86" customWidth="true" style="1" width="13.140625" collapsed="true"/>
-    <col min="87" max="87" customWidth="true" style="2" width="12.0" collapsed="true"/>
-    <col min="88" max="88" customWidth="true" style="2" width="13.28515625" collapsed="true"/>
-    <col min="89" max="89" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
-    <col min="90" max="90" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="91" max="91" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
-    <col min="92" max="92" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
-    <col min="93" max="93" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="94" max="94" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
-    <col min="95" max="95" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
-    <col min="96" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="24" width="24.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="24" width="20.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="24" width="24.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="26" max="27" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="24" width="27.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="30" max="31" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="24" width="20.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="24" width="31.0" collapsed="true"/>
+    <col min="34" max="47" customWidth="true" style="24" width="28.140625" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="50" max="50" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" style="24" width="16.28515625" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="53" max="55" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="56" max="56" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="57" max="61" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" style="24" width="24.140625" collapsed="true"/>
+    <col min="63" max="65" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" style="24" width="25.7109375" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" style="24" width="25.140625" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" style="24" width="29.0" collapsed="true"/>
+    <col min="69" max="69" customWidth="true" style="24" width="30.7109375" collapsed="true"/>
+    <col min="70" max="70" customWidth="true" style="24" width="25.7109375" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" style="24" width="27.7109375" collapsed="true"/>
+    <col min="72" max="72" customWidth="true" style="24" width="24.0" collapsed="true"/>
+    <col min="73" max="76" customWidth="true" style="24" width="29.5703125" collapsed="true"/>
+    <col min="77" max="87" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
+    <col min="88" max="88" customWidth="true" style="24" width="26.28515625" collapsed="true"/>
+    <col min="89" max="90" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
+    <col min="91" max="94" customWidth="true" style="24" width="24.7109375" collapsed="true"/>
+    <col min="95" max="95" customWidth="true" style="24" width="30.5703125" collapsed="true"/>
+    <col min="96" max="96" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="97" max="97" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="98" max="101" customWidth="true" style="24" width="24.85546875" collapsed="true"/>
+    <col min="102" max="102" customWidth="true" style="2" width="14.0" collapsed="true"/>
+    <col min="103" max="103" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
+    <col min="104" max="104" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="105" max="105" customWidth="true" style="2" width="12.0" collapsed="true"/>
+    <col min="106" max="106" customWidth="true" style="2" width="13.28515625" collapsed="true"/>
+    <col min="107" max="107" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
+    <col min="108" max="108" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="109" max="109" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+    <col min="110" max="110" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="111" max="111" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="112" max="112" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
+    <col min="113" max="113" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
+    <col min="114" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:116">
       <c r="A1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG1" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH1" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ1" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK1" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN1" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO1" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="AS1" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="AU1" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="AV1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AW1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AX1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AY1" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AZ1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="BE1" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="BF1" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="BG1" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="BH1" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="BI1" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="BJ1" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK1" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="BL1" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="BM1" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="BN1" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="BO1" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="BP1" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ1" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="BR1" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="BS1" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT1" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="BU1" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="BV1" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="BW1" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="BX1" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="BY1" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="BZ1" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="CA1" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="CB1" s="48" t="s">
+        <v>221</v>
+      </c>
+      <c r="CC1" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="CD1" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="CE1" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="CF1" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG1" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="CH1" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="CI1" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="CJ1" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="CK1" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="CL1" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="CM1" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="CN1" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="CO1" s="48" t="s">
+        <v>199</v>
+      </c>
+      <c r="CP1" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="CQ1" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="CR1" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="CS1" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="CT1" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="CU1" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="CV1" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="CW1" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="CX1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="CY1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CZ1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="DA1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="Y1" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC1" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD1" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE1" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="AF1" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="AG1" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="AH1" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="AI1" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="AJ1" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="AK1" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="AL1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="AM1" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="AN1" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="AO1" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="AP1" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="AQ1" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="AR1" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="AS1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT1" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU1" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="AW1" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="AX1" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="AY1" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="AZ1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BA1" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="BB1" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="BC1" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="BD1" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="BE1" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="BF1" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="BG1" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="BH1" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="BI1" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="BJ1" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="BK1" s="47" t="s">
-        <v>145</v>
-      </c>
-      <c r="BL1" s="47" t="s">
-        <v>171</v>
-      </c>
-      <c r="BM1" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="BN1" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="BO1" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="BP1" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="BQ1" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="BR1" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="BS1" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="BT1" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="BU1" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="BV1" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="BW1" s="48" t="s">
-        <v>205</v>
-      </c>
-      <c r="BX1" s="48" t="s">
-        <v>207</v>
-      </c>
-      <c r="BY1" s="48" t="s">
-        <v>206</v>
-      </c>
-      <c r="BZ1" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="CA1" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="CB1" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="CC1" s="47" t="s">
-        <v>185</v>
-      </c>
-      <c r="CD1" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="CE1" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="CF1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="CG1" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="CH1" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="CI1" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="CJ1" s="20" t="s">
+      <c r="DB1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="DC1" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="CK1" s="20" t="s">
+      <c r="DD1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="DE1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="CL1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="CM1" s="20" t="s">
+      <c r="DF1" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="CN1" s="20" t="s">
+      <c r="DG1" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="CO1" s="20" t="s">
+      <c r="DH1" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="CP1" s="20" t="s">
+      <c r="DI1" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="CQ1" s="20" t="s">
+      <c r="DJ1" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="CR1" s="20" t="s">
+      <c r="DK1" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="CS1" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="CT1" s="20" t="s">
-        <v>80</v>
+      <c r="DL1" s="20" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="2" spans="1:98">
+    <row customHeight="1" ht="24" r="2" spans="1:116">
       <c r="A2" s="17">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="P2" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="17">
+        <v>0</v>
+      </c>
+      <c r="R2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="S2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="M2" s="17">
+      <c r="U2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z2" s="15">
+        <v>45000</v>
+      </c>
+      <c r="AA2" s="15">
+        <v>11250</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW2" s="15"/>
+      <c r="AX2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY2" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="AZ2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB2" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="BD2" s="15">
         <v>1</v>
       </c>
-      <c r="N2" s="17">
-        <v>0</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="15" t="s">
+      <c r="BE2" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="BF2" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="BG2" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BH2" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BI2" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BJ2" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BK2" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BL2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN2" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BO2" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="BP2" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="BQ2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR2" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="BS2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="BT2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="BU2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="BV2" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="BW2" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="BX2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="BY2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BZ2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CA2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="CB2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="CC2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="CD2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="CE2" s="15"/>
+      <c r="CF2" s="15"/>
+      <c r="CG2" s="15"/>
+      <c r="CH2" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="CI2" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="V2" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="W2" s="15">
-        <v>45000</v>
-      </c>
-      <c r="X2" s="15">
-        <v>11250</v>
-      </c>
-      <c r="Y2" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD2" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE2" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AH2" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AI2" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AJ2" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AK2" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AL2" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AM2" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AN2" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AO2" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP2" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ2" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR2" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AS2" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="AW2" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX2" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AZ2" s="15">
-        <v>1</v>
-      </c>
-      <c r="BA2" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="BB2" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="BC2" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="BD2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BE2" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="BF2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="BG2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="BH2" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="BI2" s="15" t="s">
+      <c r="CJ2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CK2" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="CL2" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="CM2" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="CN2" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="CO2" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP2" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="CQ2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CR2" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="CS2" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="CT2" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="BJ2" s="15" t="s">
+      <c r="CU2" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="BK2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BL2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BM2" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="BN2" s="15"/>
-      <c r="BO2" s="15"/>
-      <c r="BP2" s="15"/>
-      <c r="BQ2" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="BR2" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="BS2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BT2" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="BU2" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="BV2" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="BW2" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="BX2" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="BY2" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="BZ2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="CA2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="CB2" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="CC2" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="CD2" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="CE2" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="CF2" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="CG2" s="15" t="s">
+      <c r="CV2" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="CW2" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="CX2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="CY2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="CZ2" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="CH2" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="CI2" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="CJ2" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="CK2" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="CL2" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="CM2" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="CN2" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="CO2" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="CP2" s="18"/>
-      <c r="CQ2" s="18"/>
-      <c r="CR2" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="CS2" s="18"/>
-      <c r="CT2" s="18" t="s">
-        <v>201</v>
+      <c r="DA2" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="DB2" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="DC2" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="DD2" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="DE2" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="DF2" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="DG2" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="DH2" s="18"/>
+      <c r="DI2" s="18"/>
+      <c r="DJ2" s="18"/>
+      <c r="DK2" s="18"/>
+      <c r="DL2" s="18" t="s">
+        <v>258</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="3" spans="1:98">
+    <row customHeight="1" ht="24" r="3" spans="1:116">
       <c r="A3" s="17">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="P3" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="17">
+        <v>1</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z3" s="15">
+        <v>45000</v>
+      </c>
+      <c r="AA3" s="15">
+        <v>11250</v>
+      </c>
+      <c r="AB3" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH3" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV3" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="AW3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AX3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY3" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="AZ3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC3" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="BD3" s="15">
+        <v>1</v>
+      </c>
+      <c r="BE3" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="BF3" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="BG3" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BH3" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BI3" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BJ3" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BK3" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BL3" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM3" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN3" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BO3" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="BP3" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="BQ3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR3" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="BS3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="BT3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="BU3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="BV3" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="BW3" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="BX3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="BY3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BZ3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CA3" s="15"/>
+      <c r="CB3" s="15"/>
+      <c r="CC3" s="15"/>
+      <c r="CD3" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="CE3" s="15"/>
+      <c r="CF3" s="15"/>
+      <c r="CG3" s="15"/>
+      <c r="CH3" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="CI3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="CJ3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CK3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="CL3" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="CM3" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="CN3" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="CO3" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP3" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="CQ3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CR3" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="CS3" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="CT3" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="CU3" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="CV3" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="CW3" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="CX3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="CY3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="CZ3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="DA3" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="DB3" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="DC3" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="DD3" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="DE3" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="DF3" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="DG3" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="DH3" s="18"/>
+      <c r="DI3" s="18"/>
+      <c r="DJ3" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="DK3" s="18"/>
+      <c r="DL3" s="18"/>
+    </row>
+    <row customHeight="1" ht="24" r="4" spans="1:116">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="P4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>1</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="W4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y4" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z4" s="15">
+        <v>45000</v>
+      </c>
+      <c r="AA4" s="15">
+        <v>11250</v>
+      </c>
+      <c r="AB4" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH4" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV4" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="AW4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AX4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY4" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="AZ4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB4" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC4" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="BD4" s="15">
+        <v>1</v>
+      </c>
+      <c r="BE4" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="BF4" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="BG4" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BH4" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BI4" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BJ4" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BK4" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BL4" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM4" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN4" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BO4" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="BP4" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="BQ4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR4" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="BS4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="BT4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="BU4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="BV4" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="BW4" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="BX4" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="BY4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BZ4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CA4" s="15"/>
+      <c r="CB4" s="15"/>
+      <c r="CC4" s="15"/>
+      <c r="CD4" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="CE4" s="15"/>
+      <c r="CF4" s="15"/>
+      <c r="CG4" s="15"/>
+      <c r="CH4" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="CI4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="CJ4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CK4" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="CL4" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="CM4" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="CN4" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="CO4" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP4" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="CQ4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CR4" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="CS4" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="CT4" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="CU4" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="CV4" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="CW4" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="CX4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="CY4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="CZ4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="DA4" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="DB4" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="DC4" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="DD4" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="DE4" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="DF4" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="DG4" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="DH4" s="18"/>
+      <c r="DI4" s="18"/>
+      <c r="DJ4" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="DK4" s="18"/>
+      <c r="DL4" s="18"/>
+    </row>
+    <row customHeight="1" ht="24" r="5" spans="1:116">
+      <c r="A5" s="17">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="13" t="s">
+      <c r="D5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="N5" s="14"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>0</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="17">
+      <c r="T5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y5" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z5" s="15">
+        <v>45000</v>
+      </c>
+      <c r="AA5" s="15">
+        <v>11250</v>
+      </c>
+      <c r="AB5" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AW5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AX5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY5" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="AZ5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC5" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="BD5" s="15">
         <v>1</v>
       </c>
-      <c r="N3" s="17">
-        <v>0</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="W3" s="15">
-        <v>45000</v>
-      </c>
-      <c r="X3" s="15">
-        <v>11250</v>
-      </c>
-      <c r="Y3" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="AE3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="AF3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AK3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AN3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AQ3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AR3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT3" s="15"/>
-      <c r="AU3" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV3" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="AW3" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX3" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY3" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AZ3" s="15">
-        <v>1</v>
-      </c>
-      <c r="BA3" s="15" t="s">
+      <c r="BE5" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF5" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="BG5" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BH5" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BI5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ5" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BK5" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BL5" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="BM5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN5" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BO5" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="BB3" s="15" t="s">
+      <c r="BP5" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="BC3" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="BD3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="BE3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BF3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BG3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BH3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BI3" s="15" t="s">
+      <c r="BQ5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="BR5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="BS5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="BT5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="BU5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV5" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="BW5" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="BX5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="BY5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BZ5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CA5" s="15"/>
+      <c r="CB5" s="15"/>
+      <c r="CC5" s="15"/>
+      <c r="CD5" s="15"/>
+      <c r="CE5" s="15"/>
+      <c r="CF5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CG5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CH5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CI5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CJ5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CK5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CL5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CM5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CN5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CO5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CP5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="CQ5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CR5" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="CS5" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="CT5" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="BJ3" s="15" t="s">
+      <c r="CU5" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="BK3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BL3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="BM3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BN3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BO3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BP3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BQ3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BR3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BS3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="BT3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BU3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BV3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BW3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BX3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BY3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BZ3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="CA3" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="CB3" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="CC3" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="CD3" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="CE3" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="CF3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="CG3" s="15" t="s">
+      <c r="CV5" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="CW5" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="CX5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="CY5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="CZ5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="CH3" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="CI3" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="CJ3" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="CK3" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="CL3" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="CM3" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="CN3" s="18"/>
-      <c r="CO3" s="18"/>
-      <c r="CP3" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="CQ3" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="CR3" s="18"/>
-      <c r="CS3" s="18"/>
-      <c r="CT3" s="18" t="s">
-        <v>204</v>
-      </c>
+      <c r="DA5" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="DB5" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="DC5" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="DD5" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="DE5" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="DF5" s="18"/>
+      <c r="DG5" s="18"/>
+      <c r="DH5" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="DI5" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="DJ5" s="18"/>
+      <c r="DK5" s="18"/>
+      <c r="DL5" s="18"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -14052,109 +14942,109 @@
   <sheetData>
     <row customFormat="1" ht="12.75" r="1" s="7" spans="1:35">
       <c r="A1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" s="37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="L1" s="26" t="s">
-        <v>119</v>
-      </c>
       <c r="M1" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N1" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="W1" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="X1" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y1" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AB1" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AC1" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="AC1" s="26" t="s">
+      <c r="AD1" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="AD1" s="26" t="s">
-        <v>99</v>
-      </c>
       <c r="AE1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="AF1" s="26" t="s">
-        <v>77</v>
-      </c>
       <c r="AG1" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AH1" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AI1" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row customFormat="1" ht="25.5" r="2" s="7" spans="1:35">
@@ -14162,97 +15052,97 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
       <c r="H2" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="J2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="K2" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="L2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="L2" s="29" t="s">
-        <v>124</v>
-      </c>
       <c r="M2" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P2" s="32"/>
       <c r="Q2" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="U2" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="V2" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="X2" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB2" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC2" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD2" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF2" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG2" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH2" s="36" t="s">
         <v>125</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="S2" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="U2" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="V2" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="W2" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="X2" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y2" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z2" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA2" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB2" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC2" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="AD2" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE2" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF2" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG2" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH2" s="36" t="s">
-        <v>126</v>
       </c>
       <c r="AI2" s="36"/>
     </row>
@@ -14265,10 +15155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F15" sqref="F1:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14278,250 +15168,323 @@
     <col min="3" max="3" customWidth="true" style="24" width="21.28515625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="24" width="21.140625" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="24" width="21.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="24" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="24" width="19.0" collapsed="true"/>
     <col min="7" max="16384" style="24" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="33" r="1" spans="1:6">
+    <row customHeight="1" ht="33" r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="19.5" r="2" s="43" spans="1:7">
+      <c r="A2" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>200</v>
+      <c r="C2" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>243</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.5" r="2" s="43" spans="1:6">
-      <c r="A2" s="41" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="41" t="s">
+    <row customFormat="1" customHeight="1" ht="46.5" r="3" s="43" spans="1:7">
+      <c r="A3" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="34.5" r="4" s="43" spans="1:7">
+      <c r="A4" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>232</v>
-      </c>
-      <c r="E2" s="45"/>
+      <c r="C4" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="46.5" r="3" s="43" spans="1:6">
-      <c r="A3" s="41" t="s">
-        <v>225</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>231</v>
-      </c>
-      <c r="E3" s="45"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="34.5" r="4" s="43" spans="1:6">
-      <c r="A4" s="41" t="s">
-        <v>226</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>231</v>
-      </c>
-      <c r="E4" s="45"/>
-    </row>
-    <row customFormat="1" r="5" s="43" spans="1:6">
+    <row customFormat="1" r="5" s="43" spans="1:7">
       <c r="A5" s="41">
         <v>91127</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>231</v>
-      </c>
-      <c r="E5" s="45"/>
+        <v>242</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row customFormat="1" r="6" s="43" spans="1:6">
+    <row customFormat="1" r="6" s="43" spans="1:7">
       <c r="A6" s="41">
         <v>91127</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>231</v>
-      </c>
-      <c r="E6" s="45"/>
+        <v>242</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row ht="45" r="7" spans="1:6">
+    <row ht="45" r="7" spans="1:7">
       <c r="A7" s="49" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E7" s="36"/>
+        <v>242</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row ht="45" r="8" spans="1:6">
+    <row ht="45" r="8" spans="1:7">
       <c r="A8" s="46">
         <v>91851</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E8" s="36"/>
+        <v>242</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row ht="45" r="9" spans="1:6">
+    <row ht="45" r="9" spans="1:7">
       <c r="A9" s="46" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E9" s="36"/>
+        <v>242</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row ht="45" r="10" spans="1:6">
+    <row ht="45" r="10" spans="1:7">
       <c r="A10" s="46">
         <v>91853</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E10" s="36"/>
+        <v>242</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row ht="30" r="11" spans="1:6">
+    <row ht="45" r="11" spans="1:7">
       <c r="A11" s="46">
         <v>91150</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="50" t="s">
-        <v>230</v>
+        <v>243</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="G11" s="50" t="s">
+        <v>217</v>
       </c>
     </row>
-    <row ht="30" r="12" spans="1:6">
+    <row ht="45" r="12" spans="1:7">
       <c r="A12" s="46">
         <v>91155</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="50" t="s">
-        <v>230</v>
+        <v>243</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>217</v>
       </c>
     </row>
-    <row ht="30" r="13" spans="1:6">
+    <row ht="45" r="13" spans="1:7">
       <c r="A13" s="46">
         <v>91155</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="50" t="s">
-        <v>230</v>
+        <v>243</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>217</v>
       </c>
     </row>
-    <row ht="30" r="14" spans="1:6">
+    <row ht="45" r="14" spans="1:7">
       <c r="A14" s="46">
         <v>91315</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="50" t="s">
-        <v>230</v>
+        <v>243</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="G14" s="50" t="s">
+        <v>217</v>
       </c>
     </row>
-    <row ht="30" r="15" spans="1:6">
+    <row ht="45" r="15" spans="1:7">
       <c r="A15" s="46">
         <v>91315</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="50" t="s">
-        <v>230</v>
+        <v>243</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on WC Business Sumary
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="7455" windowWidth="19200" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="7455" windowWidth="19200" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TD_GL" r:id="rId1" sheetId="3"/>
@@ -17,7 +17,7 @@
     <sheet name="TD_CSQ" r:id="rId3" sheetId="6"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">TD_WC!$A$1:$AI$1</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">TD_WC!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="295">
   <si>
     <t>Class Code</t>
   </si>
@@ -762,82 +762,163 @@
     <t>EW-866896</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Producer Fee</t>
+  </si>
+  <si>
+    <t>Description Of Business</t>
+  </si>
+  <si>
+    <t>Years In Business</t>
+  </si>
+  <si>
+    <t>Years In Trade</t>
+  </si>
+  <si>
+    <t>Business Desc.</t>
+  </si>
+  <si>
+    <t>Sub Contractor Description</t>
+  </si>
+  <si>
+    <t>OK-Approved</t>
+  </si>
+  <si>
+    <t>04/13/2020</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>$4,091</t>
+  </si>
+  <si>
+    <t>$25</t>
+  </si>
+  <si>
+    <t>Matched/ Not Matched (TC-04)</t>
+  </si>
+  <si>
+    <t>$3,922</t>
+  </si>
+  <si>
+    <t>$90</t>
+  </si>
+  <si>
+    <t>$100</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-172414120</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>$1,235</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-726550805</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-382832460</t>
+  </si>
+  <si>
+    <t>FGFL0020334900</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-259003251</t>
+  </si>
+  <si>
+    <t>Owner / Officers Permission</t>
+  </si>
+  <si>
+    <t>Owner / Officers Count</t>
+  </si>
+  <si>
+    <t>UW Modify AI</t>
+  </si>
+  <si>
+    <t>UWFCG1001</t>
+  </si>
+  <si>
+    <t>UWCG2010</t>
+  </si>
+  <si>
+    <t>UWCG2037</t>
+  </si>
+  <si>
+    <t>UWCG1019</t>
+  </si>
+  <si>
+    <t>UWCG2404</t>
+  </si>
+  <si>
+    <t>UWCG2012</t>
+  </si>
+  <si>
+    <t>UWCG2029</t>
+  </si>
+  <si>
+    <t>UWCG2028</t>
+  </si>
+  <si>
+    <t>UWCG2024</t>
+  </si>
+  <si>
+    <t>UWCG2005</t>
+  </si>
+  <si>
+    <t>UWCG2011</t>
+  </si>
+  <si>
+    <t>UWCG2007</t>
+  </si>
+  <si>
+    <t>UWCG2026</t>
+  </si>
+  <si>
+    <t>UW Modify IM</t>
+  </si>
+  <si>
+    <t>UW Modify Schedule Equipment</t>
+  </si>
+  <si>
+    <t>UW Modify Schedule Equipment Description</t>
+  </si>
+  <si>
+    <t>UW Modify Schedule Equipment Amount</t>
+  </si>
+  <si>
+    <t>UW Modify Installation Floater</t>
+  </si>
+  <si>
+    <t>UW Modify Contractors Hand Tools</t>
+  </si>
+  <si>
+    <t>UW Modify Rented or Leased Equipment</t>
+  </si>
+  <si>
     <t>Matched</t>
   </si>
   <si>
     <t>Not Matched</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Producer Fee</t>
-  </si>
-  <si>
-    <t>Description Of Business</t>
-  </si>
-  <si>
-    <t>Years In Business</t>
-  </si>
-  <si>
-    <t>Years In Trade</t>
-  </si>
-  <si>
-    <t>Business Desc.</t>
-  </si>
-  <si>
-    <t>Sub Contractor Description</t>
-  </si>
-  <si>
-    <t>OK-Approved</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-212907442</t>
-  </si>
-  <si>
-    <t>04/13/2020</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>$4,091</t>
-  </si>
-  <si>
-    <t>$25</t>
-  </si>
-  <si>
-    <t>FGFL0020334300</t>
-  </si>
-  <si>
-    <t>Matched/ Not Matched (TC-04)</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-550105751</t>
-  </si>
-  <si>
-    <t>$3,922</t>
-  </si>
-  <si>
-    <t>$90</t>
-  </si>
-  <si>
-    <t>$100</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-172414120</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>$1,235</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-726550805</t>
+    <t>UWModifyWS</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-210966036</t>
+  </si>
+  <si>
+    <t>04/14/2020</t>
+  </si>
+  <si>
+    <t>$3,172</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1338,6 +1419,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7205,7 +7292,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -7340,6 +7427,9 @@
     </xf>
     <xf applyAlignment="1" applyFill="1" borderId="0" fillId="41" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="42" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5527">
@@ -13171,10 +13261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DM5"/>
+  <dimension ref="A1:EI5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="CU1" workbookViewId="0">
+      <selection activeCell="CY9" sqref="CY9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13229,30 +13319,40 @@
     <col min="71" max="71" customWidth="true" style="24" width="27.7109375" collapsed="true"/>
     <col min="72" max="72" customWidth="true" style="24" width="24.0" collapsed="true"/>
     <col min="73" max="76" customWidth="true" style="24" width="29.5703125" collapsed="true"/>
-    <col min="77" max="87" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
-    <col min="88" max="88" customWidth="true" style="24" width="26.28515625" collapsed="true"/>
-    <col min="89" max="90" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
-    <col min="91" max="94" customWidth="true" style="24" width="24.7109375" collapsed="true"/>
-    <col min="95" max="95" customWidth="true" style="24" width="30.5703125" collapsed="true"/>
-    <col min="96" max="96" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="97" max="97" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="98" max="101" customWidth="true" style="24" width="24.85546875" collapsed="true"/>
-    <col min="102" max="102" customWidth="true" style="2" width="14.0" collapsed="true"/>
-    <col min="103" max="103" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
-    <col min="104" max="104" customWidth="true" style="1" width="13.140625" collapsed="true"/>
-    <col min="105" max="105" customWidth="true" style="2" width="12.0" collapsed="true"/>
-    <col min="106" max="106" customWidth="true" style="2" width="13.28515625" collapsed="true"/>
-    <col min="107" max="107" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
-    <col min="108" max="108" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="109" max="109" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
-    <col min="110" max="110" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
-    <col min="111" max="111" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="112" max="112" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
-    <col min="113" max="113" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
-    <col min="114" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="77" max="88" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
+    <col min="89" max="102" customWidth="true" style="24" width="28.140625" collapsed="true"/>
+    <col min="103" max="103" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
+    <col min="104" max="104" customWidth="true" style="24" width="30.7109375" collapsed="true"/>
+    <col min="105" max="105" customWidth="true" style="24" width="33.5703125" collapsed="true"/>
+    <col min="106" max="106" customWidth="true" style="24" width="37.5703125" collapsed="true"/>
+    <col min="107" max="107" customWidth="true" style="24" width="31.85546875" collapsed="true"/>
+    <col min="108" max="108" customWidth="true" style="24" width="34.42578125" collapsed="true"/>
+    <col min="109" max="109" customWidth="true" style="24" width="36.42578125" collapsed="true"/>
+    <col min="110" max="110" customWidth="true" style="24" width="26.28515625" collapsed="true"/>
+    <col min="111" max="112" customWidth="true" style="24" width="21.7109375" collapsed="true"/>
+    <col min="113" max="114" customWidth="true" style="24" width="24.7109375" collapsed="true"/>
+    <col min="115" max="115" customWidth="true" style="24" width="31.0" collapsed="true"/>
+    <col min="116" max="116" customWidth="true" style="24" width="32.42578125" collapsed="true"/>
+    <col min="117" max="117" customWidth="true" style="24" width="30.5703125" collapsed="true"/>
+    <col min="118" max="118" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="119" max="119" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="120" max="123" customWidth="true" style="24" width="24.85546875" collapsed="true"/>
+    <col min="124" max="124" customWidth="true" style="2" width="14.0" collapsed="true"/>
+    <col min="125" max="125" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
+    <col min="126" max="126" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="127" max="127" customWidth="true" style="2" width="12.0" collapsed="true"/>
+    <col min="128" max="128" customWidth="true" style="2" width="13.28515625" collapsed="true"/>
+    <col min="129" max="129" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
+    <col min="130" max="130" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="131" max="131" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+    <col min="132" max="132" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="133" max="133" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="134" max="134" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
+    <col min="135" max="135" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
+    <col min="136" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116">
+    <row r="1" spans="1:138">
       <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
@@ -13284,10 +13384,10 @@
         <v>14</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>0</v>
@@ -13296,10 +13396,10 @@
         <v>27</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="Q1" s="11" t="s">
         <v>2</v>
@@ -13479,7 +13579,7 @@
         <v>179</v>
       </c>
       <c r="BX1" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="BY1" s="47" t="s">
         <v>144</v>
@@ -13515,94 +13615,160 @@
         <v>169</v>
       </c>
       <c r="CJ1" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="CK1" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="CL1" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="CM1" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="CN1" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="CO1" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="CP1" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="CQ1" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="CR1" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="CS1" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="CT1" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="CU1" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV1" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="CW1" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="CX1" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="CY1" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="CZ1" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="DA1" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="DB1" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="DC1" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="DD1" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="DE1" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="DF1" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="CK1" s="48" t="s">
+      <c r="DG1" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="CL1" s="48" t="s">
+      <c r="DH1" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="CM1" s="48" t="s">
+      <c r="DI1" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="CN1" s="48" t="s">
+      <c r="DJ1" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="CO1" s="48" t="s">
+      <c r="DK1" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="CP1" s="48" t="s">
+      <c r="DL1" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="CQ1" s="47" t="s">
+      <c r="DM1" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="CR1" s="47" t="s">
+      <c r="DN1" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="CS1" s="47" t="s">
+      <c r="DO1" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="CT1" s="47" t="s">
+      <c r="DP1" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="CU1" s="47" t="s">
+      <c r="DQ1" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="CV1" s="47" t="s">
+      <c r="DR1" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="CW1" s="47" t="s">
+      <c r="DS1" s="47" t="s">
         <v>218</v>
       </c>
-      <c r="CX1" s="11" t="s">
+      <c r="DT1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="CY1" s="11" t="s">
+      <c r="DU1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="CZ1" s="11" t="s">
+      <c r="DV1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="DA1" s="20" t="s">
+      <c r="DW1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="DB1" s="20" t="s">
+      <c r="DX1" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="DC1" s="20" t="s">
+      <c r="DY1" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="DD1" s="20" t="s">
+      <c r="DZ1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="DE1" s="20" t="s">
+      <c r="EA1" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="DF1" s="20" t="s">
+      <c r="EB1" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="DG1" s="20" t="s">
+      <c r="EC1" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="DH1" s="20" t="s">
+      <c r="ED1" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="DI1" s="20" t="s">
+      <c r="EE1" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="DJ1" s="20" t="s">
+      <c r="EF1" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="DK1" s="20" t="s">
+      <c r="EG1" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="DL1" s="20" t="s">
+      <c r="EH1" s="51" t="s">
         <v>79</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="2" spans="1:116">
+    <row customHeight="1" ht="24" r="2" spans="1:138">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -13628,7 +13794,7 @@
         <v>32</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>71</v>
@@ -13640,7 +13806,7 @@
         <v>163</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="P2" s="17">
         <v>0</v>
@@ -13733,7 +13899,7 @@
         <v>71</v>
       </c>
       <c r="AT2" s="15" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="AU2" s="15" t="s">
         <v>71</v>
@@ -13851,86 +14017,152 @@
         <v>64</v>
       </c>
       <c r="CJ2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CK2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="CK2" s="15" t="s">
+      <c r="CL2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CM2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CN2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CO2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CP2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CQ2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CR2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CS2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CT2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="CU2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="CV2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="CW2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="CX2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CY2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CZ2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DA2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DB2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DC2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="DD2" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="DE2" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="DF2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="DG2" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="CL2" s="15" t="s">
+      <c r="DH2" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="CM2" s="15" t="s">
+      <c r="DI2" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="CN2" s="15" t="s">
+      <c r="DJ2" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="CO2" s="15" t="s">
+      <c r="DK2" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="CP2" s="15" t="s">
+      <c r="DL2" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="CQ2" s="15" t="s">
+      <c r="DM2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="CR2" s="15" t="s">
+      <c r="DN2" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="CS2" s="15" t="s">
+      <c r="DO2" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="CT2" s="15" t="s">
+      <c r="DP2" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="CU2" s="15" t="s">
+      <c r="DQ2" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="CV2" s="15" t="s">
+      <c r="DR2" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="CW2" s="15" t="s">
+      <c r="DS2" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="CX2" s="15" t="s">
+      <c r="DT2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CY2" s="15" t="s">
+      <c r="DU2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="CZ2" s="15" t="s">
+      <c r="DV2" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="DA2" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="DB2" s="12" t="s">
+      <c r="DW2" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="DX2" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="DY2" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="DZ2" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="EA2" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="DC2" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="DD2" s="18" t="s">
+      <c r="EB2" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="EC2" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="DE2" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="DF2" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="DG2" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="DH2" s="18"/>
-      <c r="DI2" s="18"/>
-      <c r="DJ2" s="18"/>
-      <c r="DK2" s="18"/>
-      <c r="DL2" s="18" t="s">
-        <v>258</v>
+      <c r="ED2" s="18"/>
+      <c r="EE2" s="18"/>
+      <c r="EF2" s="18"/>
+      <c r="EG2" s="18"/>
+      <c r="EH2" s="18" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="3" spans="1:116">
+    <row customHeight="1" ht="24" r="3" spans="1:138">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -13956,7 +14188,7 @@
         <v>32</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L3" s="13" t="s">
         <v>71</v>
@@ -13968,7 +14200,7 @@
         <v>163</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="P3" s="17">
         <v>0</v>
@@ -14061,7 +14293,7 @@
         <v>71</v>
       </c>
       <c r="AT3" s="15" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="AU3" s="15" t="s">
         <v>71</v>
@@ -14175,86 +14407,126 @@
         <v>64</v>
       </c>
       <c r="CJ3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CK3" s="15"/>
+      <c r="CL3" s="15"/>
+      <c r="CM3" s="15"/>
+      <c r="CN3" s="15"/>
+      <c r="CO3" s="15"/>
+      <c r="CP3" s="15"/>
+      <c r="CQ3" s="15"/>
+      <c r="CR3" s="15"/>
+      <c r="CS3" s="15"/>
+      <c r="CT3" s="15"/>
+      <c r="CU3" s="15"/>
+      <c r="CV3" s="15"/>
+      <c r="CW3" s="15"/>
+      <c r="CX3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CY3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="CK3" s="15" t="s">
+      <c r="CZ3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DA3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DB3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DC3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="DD3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="DE3" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="DF3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="DG3" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="CL3" s="15" t="s">
+      <c r="DH3" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="CM3" s="15" t="s">
+      <c r="DI3" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="CN3" s="15" t="s">
+      <c r="DJ3" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="CO3" s="15" t="s">
+      <c r="DK3" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="CP3" s="15" t="s">
+      <c r="DL3" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="CQ3" s="15" t="s">
+      <c r="DM3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="CR3" s="15" t="s">
+      <c r="DN3" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="CS3" s="15" t="s">
+      <c r="DO3" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="CT3" s="15" t="s">
+      <c r="DP3" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="CU3" s="15" t="s">
+      <c r="DQ3" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="CV3" s="15" t="s">
+      <c r="DR3" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="CW3" s="15" t="s">
+      <c r="DS3" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="CX3" s="15" t="s">
+      <c r="DT3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CY3" s="15" t="s">
+      <c r="DU3" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="CZ3" s="15" t="s">
+      <c r="DV3" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="DA3" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="DB3" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="DC3" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="DD3" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="DE3" s="18" t="s">
+      <c r="DW3" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="DX3" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="DY3" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="DZ3" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="EA3" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="DF3" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="DG3" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="DH3" s="18"/>
-      <c r="DI3" s="18"/>
-      <c r="DJ3" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="DK3" s="18"/>
-      <c r="DL3" s="18"/>
+      <c r="EB3" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="EC3" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="ED3" s="18"/>
+      <c r="EE3" s="18"/>
+      <c r="EF3" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="EG3" s="18"/>
+      <c r="EH3" s="18"/>
     </row>
-    <row customHeight="1" ht="24" r="4" spans="1:116">
+    <row customHeight="1" ht="24" r="4" spans="1:138">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -14280,7 +14552,7 @@
         <v>32</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>93</v>
@@ -14292,7 +14564,7 @@
         <v>163</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="P4" s="17">
         <v>1</v>
@@ -14385,7 +14657,7 @@
         <v>71</v>
       </c>
       <c r="AT4" s="15" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="AU4" s="15" t="s">
         <v>71</v>
@@ -14501,84 +14773,148 @@
       <c r="CJ4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="CK4" s="15" t="s">
+      <c r="CK4" s="15"/>
+      <c r="CL4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CM4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CN4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CO4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CP4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CQ4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CR4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CS4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CT4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="CU4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="CV4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="CW4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="CX4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CY4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="CZ4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DA4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DB4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DC4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="DD4" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="DE4" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="DF4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="DG4" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="CL4" s="15" t="s">
+      <c r="DH4" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="CM4" s="15" t="s">
+      <c r="DI4" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="CN4" s="15" t="s">
+      <c r="DJ4" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="CO4" s="15" t="s">
+      <c r="DK4" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="CP4" s="15" t="s">
+      <c r="DL4" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="CQ4" s="15" t="s">
+      <c r="DM4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="CR4" s="15" t="s">
+      <c r="DN4" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="CS4" s="15" t="s">
+      <c r="DO4" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="CT4" s="15" t="s">
+      <c r="DP4" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="CU4" s="15" t="s">
+      <c r="DQ4" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="CV4" s="15" t="s">
+      <c r="DR4" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="CW4" s="15" t="s">
+      <c r="DS4" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="CX4" s="15" t="s">
+      <c r="DT4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CY4" s="15" t="s">
+      <c r="DU4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="CZ4" s="15" t="s">
+      <c r="DV4" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="DA4" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="DB4" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="DC4" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="DD4" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="DE4" s="18" t="s">
+      <c r="DW4" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="DX4" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="DY4" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="DZ4" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="EA4" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="DF4" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="DG4" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="DH4" s="18"/>
-      <c r="DI4" s="18"/>
-      <c r="DJ4" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="DK4" s="18"/>
-      <c r="DL4" s="18"/>
+      <c r="EB4" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="EC4" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="ED4" s="18"/>
+      <c r="EE4" s="18"/>
+      <c r="EF4" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="EG4" s="18"/>
+      <c r="EH4" s="18"/>
     </row>
-    <row customHeight="1" ht="24" r="5" spans="1:116">
+    <row customHeight="1" ht="24" r="5" spans="1:138">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -14604,7 +14940,7 @@
         <v>62</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L5" s="13" t="s">
         <v>71</v>
@@ -14705,7 +15041,7 @@
         <v>93</v>
       </c>
       <c r="AT5" s="15" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="AU5" s="15" t="s">
         <v>93</v>
@@ -14824,79 +15160,145 @@
         <v>19</v>
       </c>
       <c r="CK5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CL5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CM5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CN5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CO5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CP5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CR5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CS5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CU5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CV5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CW5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CX5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CY5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CZ5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DA5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DB5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="DC5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="DD5" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="CL5" s="15" t="s">
+      <c r="DE5" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="CM5" s="15" t="s">
+      <c r="DF5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="DG5" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="CN5" s="15" t="s">
+      <c r="DH5" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="CO5" s="15" t="s">
+      <c r="DI5" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="CP5" s="15" t="s">
+      <c r="DJ5" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="CQ5" s="15" t="s">
+      <c r="DK5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="DL5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="DM5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="CR5" s="15" t="s">
+      <c r="DN5" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="CS5" s="15" t="s">
+      <c r="DO5" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="CT5" s="15" t="s">
+      <c r="DP5" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="CU5" s="15" t="s">
+      <c r="DQ5" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="CV5" s="15" t="s">
+      <c r="DR5" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="CW5" s="15" t="s">
+      <c r="DS5" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="CX5" s="15" t="s">
+      <c r="DT5" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="CY5" s="15" t="s">
+      <c r="DU5" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="CZ5" s="15" t="s">
+      <c r="DV5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="DA5" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="DB5" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="DC5" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="DD5" s="18" t="s">
+      <c r="DW5" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="DX5" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="DY5" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="DZ5" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="EA5" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="EB5" s="18"/>
+      <c r="EC5" s="18"/>
+      <c r="ED5" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="EE5" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="DE5" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="DF5" s="18"/>
-      <c r="DG5" s="18"/>
-      <c r="DH5" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="DI5" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="DJ5" s="18"/>
-      <c r="DK5" s="18"/>
-      <c r="DL5" s="18"/>
+      <c r="EF5" s="18"/>
+      <c r="EG5" s="18"/>
+      <c r="EH5" s="18"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -14906,10 +15308,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14924,23 +15326,26 @@
     <col min="13" max="14" customWidth="true" width="25.7109375" collapsed="true"/>
     <col min="15" max="15" customWidth="true" width="29.5703125" collapsed="true"/>
     <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="17" max="21" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="2" width="19.5703125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="2" width="15.0" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="17" max="20" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="24" width="23.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="24" width="22.85546875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="2" width="19.5703125" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="2" width="15.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="21.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="12.75" r="1" s="7" spans="1:35">
+    <row customFormat="1" ht="12.75" r="1" s="7" spans="1:37">
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
@@ -15002,52 +15407,58 @@
         <v>42</v>
       </c>
       <c r="U1" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="W1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="X1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="Y1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AC1" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AD1" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="AC1" s="26" t="s">
+      <c r="AE1" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="AD1" s="26" t="s">
+      <c r="AF1" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AG1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="AF1" s="26" t="s">
+      <c r="AH1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="AG1" s="35" t="s">
+      <c r="AI1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="AH1" s="35" t="s">
+      <c r="AJ1" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" s="35" t="s">
+      <c r="AK1" s="35" t="s">
         <v>79</v>
       </c>
     </row>
-    <row customFormat="1" ht="25.5" r="2" s="7" spans="1:35">
+    <row customFormat="1" ht="25.5" r="2" s="7" spans="1:37">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -15102,52 +15513,58 @@
       <c r="T2" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="U2" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="W2" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="V2" s="31" t="s">
+      <c r="X2" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="W2" s="33" t="s">
+      <c r="Y2" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="X2" s="31" t="s">
+      <c r="Z2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="31" t="s">
+      <c r="AA2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="Z2" s="31" t="s">
+      <c r="AB2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="AA2" s="31" t="s">
+      <c r="AC2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="AB2" s="34" t="s">
+      <c r="AD2" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AE2" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="AD2" s="31" t="s">
+      <c r="AF2" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AE2" s="32" t="s">
+      <c r="AG2" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="AF2" s="32" t="s">
+      <c r="AH2" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="AG2" s="36" t="s">
+      <c r="AI2" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="AH2" s="36" t="s">
+      <c r="AJ2" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="AI2" s="36"/>
+      <c r="AK2" s="36"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI1"/>
+  <autoFilter ref="A1:AK1"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -15157,8 +15574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F15" sqref="F1:F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15189,7 +15606,7 @@
         <v>195</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="19.5" r="2" s="43" spans="1:7">
@@ -15200,17 +15617,11 @@
         <v>82</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="F2" s="45" t="s">
-        <v>243</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row customFormat="1" customHeight="1" ht="46.5" r="3" s="43" spans="1:7">
       <c r="A3" s="41" t="s">
@@ -15220,17 +15631,11 @@
         <v>162</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>242</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="F3" s="45" t="s">
-        <v>242</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
     </row>
     <row customFormat="1" customHeight="1" ht="34.5" r="4" s="43" spans="1:7">
       <c r="A4" s="41" t="s">
@@ -15240,17 +15645,11 @@
         <v>83</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>242</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="F4" s="45" t="s">
-        <v>242</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row customFormat="1" r="5" s="43" spans="1:7">
       <c r="A5" s="41">
@@ -15260,17 +15659,11 @@
         <v>146</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="F5" s="45" t="s">
-        <v>242</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
     </row>
     <row customFormat="1" r="6" s="43" spans="1:7">
       <c r="A6" s="41">
@@ -15280,17 +15673,11 @@
         <v>161</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>242</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
     </row>
     <row ht="45" r="7" spans="1:7">
       <c r="A7" s="49" t="s">
@@ -15300,17 +15687,11 @@
         <v>164</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row ht="45" r="8" spans="1:7">
       <c r="A8" s="46">
@@ -15320,17 +15701,11 @@
         <v>165</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
     </row>
     <row ht="45" r="9" spans="1:7">
       <c r="A9" s="46" t="s">
@@ -15340,17 +15715,11 @@
         <v>192</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
     </row>
     <row ht="45" r="10" spans="1:7">
       <c r="A10" s="46">
@@ -15360,17 +15729,11 @@
         <v>190</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
     </row>
     <row ht="45" r="11" spans="1:7">
       <c r="A11" s="46">
@@ -15380,17 +15743,11 @@
         <v>210</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="50" t="s">
         <v>217</v>
       </c>
@@ -15403,17 +15760,11 @@
         <v>211</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="E12" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="50" t="s">
         <v>217</v>
       </c>
@@ -15426,17 +15777,11 @@
         <v>210</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="50" t="s">
         <v>217</v>
       </c>
@@ -15449,17 +15794,11 @@
         <v>215</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="50" t="s">
         <v>217</v>
       </c>
@@ -15472,17 +15811,11 @@
         <v>216</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="F15" s="36" t="s">
-        <v>243</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="50" t="s">
         <v>217</v>
       </c>

</xml_diff>

<commit_message>
Business Summary Scripting in Progress
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="301">
   <si>
     <t>Class Code</t>
   </si>
@@ -239,9 +239,6 @@
     <t>0.89</t>
   </si>
   <si>
-    <t>Mishra</t>
-  </si>
-  <si>
     <t>1,00,000</t>
   </si>
   <si>
@@ -333,9 +330,6 @@
   </si>
   <si>
     <t>Address 1</t>
-  </si>
-  <si>
-    <t>Siddharth</t>
   </si>
   <si>
     <t>187200</t>
@@ -795,9 +789,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>$4,091</t>
-  </si>
-  <si>
     <t>$25</t>
   </si>
   <si>
@@ -813,9 +804,6 @@
     <t>$100</t>
   </si>
   <si>
-    <t>FCGA AUTM-172414120</t>
-  </si>
-  <si>
     <t>06</t>
   </si>
   <si>
@@ -825,9 +813,6 @@
     <t>FCGA AUTM-726550805</t>
   </si>
   <si>
-    <t>FCGA AUTM-382832460</t>
-  </si>
-  <si>
     <t>FGFL0020334900</t>
   </si>
   <si>
@@ -912,13 +897,46 @@
     <t>UWModifyWS</t>
   </si>
   <si>
-    <t>FCGA AUTM-210966036</t>
-  </si>
-  <si>
-    <t>04/14/2020</t>
-  </si>
-  <si>
     <t>$3,172</t>
+  </si>
+  <si>
+    <t>04/15/2020</t>
+  </si>
+  <si>
+    <t>Siddharth / Rahul/ Anuyesh</t>
+  </si>
+  <si>
+    <t>Mishra/ Sharma / Kumar</t>
+  </si>
+  <si>
+    <t>33/33/34</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-628262323</t>
+  </si>
+  <si>
+    <t>BGFL0020336500</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-060914723</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-570803675</t>
+  </si>
+  <si>
+    <t>FGFL0020337100</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-086919581</t>
+  </si>
+  <si>
+    <t>BGFL0020337200</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-061485317</t>
+  </si>
+  <si>
+    <t>$3,796</t>
   </si>
 </sst>
 </file>
@@ -13263,8 +13281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EI5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CU1" workbookViewId="0">
-      <selection activeCell="CY9" sqref="CY9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13369,13 +13387,13 @@
         <v>23</v>
       </c>
       <c r="F1" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>113</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>115</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>13</v>
@@ -13384,10 +13402,10 @@
         <v>14</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>0</v>
@@ -13396,10 +13414,10 @@
         <v>27</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Q1" s="11" t="s">
         <v>2</v>
@@ -13432,10 +13450,10 @@
         <v>11</v>
       </c>
       <c r="AA1" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AB1" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AC1" s="11" t="s">
         <v>28</v>
@@ -13447,52 +13465,52 @@
         <v>30</v>
       </c>
       <c r="AF1" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG1" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH1" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="AG1" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH1" s="11" t="s">
-        <v>128</v>
-      </c>
       <c r="AI1" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ1" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK1" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AL1" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AM1" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AN1" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="AR1" s="11" t="s">
+      <c r="AT1" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AU1" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="AT1" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="AU1" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="AV1" s="11" t="s">
         <v>51</v>
@@ -13501,10 +13519,10 @@
         <v>52</v>
       </c>
       <c r="AX1" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AY1" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AZ1" s="11" t="s">
         <v>53</v>
@@ -13522,250 +13540,250 @@
         <v>12</v>
       </c>
       <c r="BE1" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="BF1" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="BG1" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="BF1" s="11" t="s">
+      <c r="BH1" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="BG1" s="11" t="s">
+      <c r="BI1" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="BH1" s="11" t="s">
+      <c r="BJ1" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="BI1" s="11" t="s">
+      <c r="BK1" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="BJ1" s="11" t="s">
+      <c r="BL1" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="BK1" s="11" t="s">
+      <c r="BM1" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="BL1" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="BM1" s="11" t="s">
-        <v>233</v>
-      </c>
       <c r="BN1" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="BO1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="BP1" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="BO1" s="11" t="s">
+      <c r="BQ1" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="BP1" s="11" t="s">
+      <c r="BR1" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="BQ1" s="11" t="s">
+      <c r="BS1" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="BR1" s="11" t="s">
+      <c r="BT1" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="BS1" s="11" t="s">
+      <c r="BU1" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="BT1" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="BU1" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="BV1" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="BW1" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="BX1" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="BY1" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="BZ1" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="CA1" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="CB1" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="CC1" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="CD1" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="CE1" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="CF1" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="CG1" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="CH1" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="CI1" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="CJ1" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="CK1" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="CL1" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="CM1" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="CN1" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="CO1" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="CP1" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="CQ1" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="CR1" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="CS1" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="CT1" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="CU1" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="CV1" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="CW1" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="CX1" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="CY1" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="CZ1" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="DA1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="DB1" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="DC1" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="DD1" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="DE1" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="DF1" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="DG1" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="DH1" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="DI1" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="DJ1" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="DK1" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="DL1" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="DM1" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="DN1" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="DO1" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="DP1" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="BW1" s="11" t="s">
+      <c r="DQ1" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="BX1" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="BY1" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="BZ1" s="47" t="s">
-        <v>166</v>
-      </c>
-      <c r="CA1" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="CB1" s="48" t="s">
-        <v>221</v>
-      </c>
-      <c r="CC1" s="48" t="s">
-        <v>222</v>
-      </c>
-      <c r="CD1" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="CE1" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="CF1" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="CG1" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="CH1" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="CI1" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="CJ1" s="47" t="s">
-        <v>268</v>
-      </c>
-      <c r="CK1" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="CL1" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="CM1" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="CN1" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="CO1" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="CP1" s="20" t="s">
-        <v>274</v>
-      </c>
-      <c r="CQ1" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="CR1" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="CS1" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="CT1" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="CU1" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="CV1" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="CW1" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="CX1" s="47" t="s">
-        <v>291</v>
-      </c>
-      <c r="CY1" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="CZ1" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="DA1" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="DB1" s="20" t="s">
-        <v>288</v>
-      </c>
-      <c r="DC1" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="DD1" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="DE1" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="DF1" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="DG1" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="DH1" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="DI1" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="DJ1" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="DK1" s="48" t="s">
-        <v>199</v>
-      </c>
-      <c r="DL1" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="DM1" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="DN1" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="DO1" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="DP1" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="DQ1" s="47" t="s">
-        <v>181</v>
-      </c>
       <c r="DR1" s="47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="DS1" s="47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="DT1" s="11" t="s">
         <v>17</v>
       </c>
       <c r="DU1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="DV1" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="DV1" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="DW1" s="51" t="s">
         <v>24</v>
       </c>
       <c r="DX1" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="DY1" s="51" t="s">
         <v>84</v>
-      </c>
-      <c r="DY1" s="51" t="s">
-        <v>85</v>
       </c>
       <c r="DZ1" s="51" t="s">
         <v>1</v>
       </c>
       <c r="EA1" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="EB1" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="EB1" s="51" t="s">
+      <c r="EC1" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="EC1" s="51" t="s">
+      <c r="ED1" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="ED1" s="51" t="s">
+      <c r="EE1" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="EE1" s="51" t="s">
+      <c r="EF1" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="EF1" s="51" t="s">
+      <c r="EG1" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="EG1" s="51" t="s">
-        <v>92</v>
-      </c>
       <c r="EH1" s="51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row customHeight="1" ht="24" r="2" spans="1:138">
@@ -13776,7 +13794,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>31</v>
@@ -13794,19 +13812,19 @@
         <v>32</v>
       </c>
       <c r="K2" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="O2" s="13" t="s">
         <v>247</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>249</v>
       </c>
       <c r="P2" s="17">
         <v>0</v>
@@ -13833,10 +13851,10 @@
         <v>16</v>
       </c>
       <c r="X2" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Y2" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Z2" s="15">
         <v>45000</v>
@@ -13845,7 +13863,7 @@
         <v>11250</v>
       </c>
       <c r="AB2" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AC2" s="15" t="s">
         <v>38</v>
@@ -13860,49 +13878,49 @@
         <v>16</v>
       </c>
       <c r="AG2" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AH2" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AI2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="AJ2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AK2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AL2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AM2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AN2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AO2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AP2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AQ2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AR2" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AS2" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AT2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="AU2" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AV2" s="15" t="s">
         <v>57</v>
@@ -13912,7 +13930,7 @@
         <v>37</v>
       </c>
       <c r="AY2" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AZ2" s="15" t="s">
         <v>58</v>
@@ -13930,46 +13948,46 @@
         <v>1</v>
       </c>
       <c r="BE2" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="BF2" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="BG2" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="BF2" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="BG2" s="15" t="s">
-        <v>238</v>
-      </c>
       <c r="BH2" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI2" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BJ2" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BK2" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BL2" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BM2" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BN2" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="BO2" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP2" s="15" t="s">
         <v>156</v>
-      </c>
-      <c r="BO2" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="BP2" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="BQ2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="BR2" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="BS2" s="15" t="s">
         <v>39</v>
@@ -13981,13 +13999,13 @@
         <v>59</v>
       </c>
       <c r="BV2" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="BW2" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="BX2" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BY2" s="15" t="s">
         <v>16</v>
@@ -14011,7 +14029,7 @@
       <c r="CF2" s="15"/>
       <c r="CG2" s="15"/>
       <c r="CH2" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="CI2" s="15" t="s">
         <v>64</v>
@@ -14023,40 +14041,40 @@
         <v>16</v>
       </c>
       <c r="CL2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CM2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CN2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CO2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CP2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CQ2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CR2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CS2" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CT2" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CU2" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CV2" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CW2" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CX2" s="15" t="s">
         <v>16</v>
@@ -14077,89 +14095,89 @@
         <v>16</v>
       </c>
       <c r="DD2" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="DE2" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="DF2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="DG2" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="DH2" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="DI2" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="DJ2" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="DK2" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="DL2" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="DM2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="DN2" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="DO2" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="DP2" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="DQ2" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="DR2" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="DS2" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="DT2" s="15" t="s">
         <v>49</v>
       </c>
       <c r="DU2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="DV2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="DV2" s="15" t="s">
-        <v>78</v>
-      </c>
       <c r="DW2" s="12" t="s">
-        <v>242</v>
+        <v>110</v>
       </c>
       <c r="DX2" s="12" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="DY2" s="8" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="DZ2" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="EA2" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="EB2" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="EC2" s="18" t="s">
         <v>251</v>
-      </c>
-      <c r="EA2" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="EB2" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="EC2" s="18" t="s">
-        <v>254</v>
       </c>
       <c r="ED2" s="18"/>
       <c r="EE2" s="18"/>
       <c r="EF2" s="18"/>
       <c r="EG2" s="18"/>
       <c r="EH2" s="18" t="s">
-        <v>264</v>
+        <v>296</v>
       </c>
     </row>
     <row customHeight="1" ht="24" r="3" spans="1:138">
@@ -14170,7 +14188,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>31</v>
@@ -14182,31 +14200,27 @@
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
       <c r="I3" s="13" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>249</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="N3" s="14"/>
+      <c r="O3" s="13"/>
       <c r="P3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="17">
         <v>0</v>
-      </c>
-      <c r="Q3" s="17">
-        <v>1</v>
       </c>
       <c r="R3" s="15" t="s">
         <v>16</v>
@@ -14215,10 +14229,10 @@
         <v>63</v>
       </c>
       <c r="T3" s="15" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="U3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="V3" s="15" t="s">
         <v>16</v>
@@ -14227,10 +14241,10 @@
         <v>16</v>
       </c>
       <c r="X3" s="19" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="Y3" s="19" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="Z3" s="15">
         <v>45000</v>
@@ -14239,7 +14253,7 @@
         <v>11250</v>
       </c>
       <c r="AB3" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AC3" s="15" t="s">
         <v>38</v>
@@ -14251,55 +14265,55 @@
         <v>38</v>
       </c>
       <c r="AF3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AG3" s="15" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="AH3" s="15" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="AI3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AJ3" s="15" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="AK3" s="15" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="AL3" s="15" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="AM3" s="15" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="AN3" s="15" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="AO3" s="15" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="AP3" s="15" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="AQ3" s="15" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="AR3" s="15" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="AS3" s="15" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="AT3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AU3" s="15" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="AV3" s="15" t="s">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="AW3" s="15" t="s">
         <v>40</v>
@@ -14308,13 +14322,13 @@
         <v>37</v>
       </c>
       <c r="AY3" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AZ3" s="15" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="BA3" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="BB3" s="15" t="s">
         <v>60</v>
@@ -14326,107 +14340,135 @@
         <v>1</v>
       </c>
       <c r="BE3" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF3" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="BG3" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="BF3" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="BG3" s="15" t="s">
-        <v>238</v>
-      </c>
       <c r="BH3" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="BI3" s="15" t="s">
-        <v>239</v>
+        <v>92</v>
       </c>
       <c r="BJ3" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="BK3" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="BL3" s="15" t="s">
-        <v>93</v>
+        <v>236</v>
       </c>
       <c r="BM3" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BN3" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="BO3" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP3" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="BO3" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="BP3" s="15" t="s">
-        <v>158</v>
-      </c>
       <c r="BQ3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="BR3" s="15" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="BS3" s="15" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="BT3" s="15" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="BU3" s="15" t="s">
-        <v>59</v>
+        <v>143</v>
       </c>
       <c r="BV3" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="BW3" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="BX3" s="15" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="BY3" s="15" t="s">
         <v>16</v>
       </c>
       <c r="BZ3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="CA3" s="15"/>
       <c r="CB3" s="15"/>
       <c r="CC3" s="15"/>
-      <c r="CD3" s="13" t="s">
-        <v>205</v>
-      </c>
+      <c r="CD3" s="15"/>
       <c r="CE3" s="15"/>
-      <c r="CF3" s="15"/>
-      <c r="CG3" s="15"/>
+      <c r="CF3" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="CG3" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="CH3" s="15" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="CI3" s="15" t="s">
-        <v>64</v>
+        <v>143</v>
       </c>
       <c r="CJ3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="CK3" s="15"/>
-      <c r="CL3" s="15"/>
-      <c r="CM3" s="15"/>
-      <c r="CN3" s="15"/>
-      <c r="CO3" s="15"/>
-      <c r="CP3" s="15"/>
-      <c r="CQ3" s="15"/>
-      <c r="CR3" s="15"/>
-      <c r="CS3" s="15"/>
-      <c r="CT3" s="15"/>
-      <c r="CU3" s="15"/>
-      <c r="CV3" s="15"/>
-      <c r="CW3" s="15"/>
+      <c r="CK3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="CL3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CM3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CN3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CO3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CQ3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CR3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CS3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CT3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CU3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CV3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="CW3" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="CX3" s="15" t="s">
         <v>19</v>
       </c>
       <c r="CY3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="CZ3" s="15" t="s">
         <v>38</v>
@@ -14438,93 +14480,93 @@
         <v>38</v>
       </c>
       <c r="DC3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="DD3" s="15" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="DE3" s="15" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="DF3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="DG3" s="15" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="DH3" s="15" t="s">
-        <v>189</v>
+        <v>143</v>
       </c>
       <c r="DI3" s="15" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="DJ3" s="15" t="s">
-        <v>206</v>
+        <v>143</v>
       </c>
       <c r="DK3" s="15" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="DL3" s="15" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
       <c r="DM3" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="DN3" s="15" t="s">
         <v>105</v>
       </c>
       <c r="DO3" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="DP3" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="DQ3" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="DR3" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="DS3" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="DT3" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="DU3" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="DV3" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="DV3" s="15" t="s">
-        <v>78</v>
-      </c>
       <c r="DW3" s="12" t="s">
-        <v>242</v>
+        <v>110</v>
       </c>
       <c r="DX3" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="DY3" s="8" t="s">
-        <v>250</v>
+        <v>297</v>
+      </c>
+      <c r="DY3" s="22" t="s">
+        <v>288</v>
       </c>
       <c r="DZ3" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="EA3" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="EB3" s="18"/>
+      <c r="EC3" s="18"/>
+      <c r="ED3" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="EE3" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="EA3" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="EB3" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="EC3" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="ED3" s="18"/>
-      <c r="EE3" s="18"/>
-      <c r="EF3" s="18" t="s">
-        <v>258</v>
-      </c>
+      <c r="EF3" s="18"/>
       <c r="EG3" s="18"/>
-      <c r="EH3" s="18"/>
+      <c r="EH3" s="18" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row customHeight="1" ht="24" r="4" spans="1:138">
       <c r="A4" s="17">
@@ -14534,7 +14576,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>31</v>
@@ -14552,22 +14594,22 @@
         <v>32</v>
       </c>
       <c r="K4" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="O4" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="L4" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>249</v>
-      </c>
       <c r="P4" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="17">
         <v>1</v>
@@ -14591,10 +14633,10 @@
         <v>16</v>
       </c>
       <c r="X4" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Y4" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Z4" s="15">
         <v>45000</v>
@@ -14603,7 +14645,7 @@
         <v>11250</v>
       </c>
       <c r="AB4" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AC4" s="15" t="s">
         <v>38</v>
@@ -14618,52 +14660,52 @@
         <v>16</v>
       </c>
       <c r="AG4" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AH4" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AI4" s="15" t="s">
         <v>16</v>
       </c>
       <c r="AJ4" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AK4" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AL4" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AM4" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AN4" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AO4" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AP4" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AQ4" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AR4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AS4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AT4" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AU4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AV4" s="15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AW4" s="15" t="s">
         <v>40</v>
@@ -14672,7 +14714,7 @@
         <v>37</v>
       </c>
       <c r="AY4" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AZ4" s="15" t="s">
         <v>58</v>
@@ -14690,46 +14732,46 @@
         <v>1</v>
       </c>
       <c r="BE4" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="BF4" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BG4" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="BF4" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="BG4" s="15" t="s">
-        <v>238</v>
-      </c>
       <c r="BH4" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI4" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BJ4" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BK4" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BL4" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BM4" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BN4" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="BO4" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP4" s="15" t="s">
         <v>156</v>
-      </c>
-      <c r="BO4" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="BP4" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="BQ4" s="15" t="s">
         <v>16</v>
       </c>
       <c r="BR4" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="BS4" s="15" t="s">
         <v>39</v>
@@ -14741,13 +14783,13 @@
         <v>59</v>
       </c>
       <c r="BV4" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="BW4" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="BX4" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BY4" s="15" t="s">
         <v>16</v>
@@ -14759,57 +14801,33 @@
       <c r="CB4" s="15"/>
       <c r="CC4" s="15"/>
       <c r="CD4" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="CE4" s="15"/>
       <c r="CF4" s="15"/>
       <c r="CG4" s="15"/>
       <c r="CH4" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="CI4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="CJ4" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="CK4" s="15"/>
-      <c r="CL4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="CM4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="CN4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="CO4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="CP4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="CQ4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="CR4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="CS4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="CT4" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="CU4" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="CV4" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="CW4" s="15" t="s">
-        <v>71</v>
-      </c>
+      <c r="CL4" s="15"/>
+      <c r="CM4" s="15"/>
+      <c r="CN4" s="15"/>
+      <c r="CO4" s="15"/>
+      <c r="CP4" s="15"/>
+      <c r="CQ4" s="15"/>
+      <c r="CR4" s="15"/>
+      <c r="CS4" s="15"/>
+      <c r="CT4" s="15"/>
+      <c r="CU4" s="15"/>
+      <c r="CV4" s="15"/>
+      <c r="CW4" s="15"/>
       <c r="CX4" s="15" t="s">
         <v>19</v>
       </c>
@@ -14829,87 +14847,87 @@
         <v>16</v>
       </c>
       <c r="DD4" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="DE4" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="DF4" s="15" t="s">
         <v>16</v>
       </c>
       <c r="DG4" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="DH4" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="DI4" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="DJ4" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="DK4" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="DL4" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="DM4" s="15" t="s">
         <v>16</v>
       </c>
       <c r="DN4" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="DO4" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="DP4" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="DQ4" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="DR4" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="DS4" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="DT4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="DU4" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="DV4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="DV4" s="15" t="s">
-        <v>78</v>
-      </c>
       <c r="DW4" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="DX4" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="DY4" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="DZ4" s="18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="EA4" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="EB4" s="18" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="EC4" s="18" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="ED4" s="18"/>
       <c r="EE4" s="18"/>
       <c r="EF4" s="18" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="EG4" s="18"/>
       <c r="EH4" s="18"/>
@@ -14922,7 +14940,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>31</v>
@@ -14930,31 +14948,35 @@
       <c r="E5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="13" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="K5" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="O5" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="13"/>
       <c r="P5" s="17">
         <v>1</v>
       </c>
       <c r="Q5" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="15" t="s">
         <v>16</v>
@@ -14963,10 +14985,10 @@
         <v>63</v>
       </c>
       <c r="T5" s="15" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="V5" s="15" t="s">
         <v>16</v>
@@ -14975,10 +14997,10 @@
         <v>16</v>
       </c>
       <c r="X5" s="19" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="Y5" s="19" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="Z5" s="15">
         <v>45000</v>
@@ -14987,7 +15009,7 @@
         <v>11250</v>
       </c>
       <c r="AB5" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AC5" s="15" t="s">
         <v>38</v>
@@ -14999,55 +15021,55 @@
         <v>38</v>
       </c>
       <c r="AF5" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AG5" s="15" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="AH5" s="15" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="AI5" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AJ5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="AK5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="AL5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="AM5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="AN5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="AO5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="AP5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="AQ5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="AR5" s="15" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="AS5" s="15" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="AT5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="AU5" s="15" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="AV5" s="15" t="s">
-        <v>39</v>
+        <v>238</v>
       </c>
       <c r="AW5" s="15" t="s">
         <v>40</v>
@@ -15056,13 +15078,13 @@
         <v>37</v>
       </c>
       <c r="AY5" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AZ5" s="15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="BA5" s="15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="BB5" s="15" t="s">
         <v>60</v>
@@ -15074,135 +15096,131 @@
         <v>1</v>
       </c>
       <c r="BE5" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="BF5" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="BG5" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="BH5" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="BF5" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="BG5" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="BH5" s="15" t="s">
-        <v>238</v>
-      </c>
       <c r="BI5" s="15" t="s">
-        <v>93</v>
+        <v>237</v>
       </c>
       <c r="BJ5" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="BK5" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="BL5" s="15" t="s">
-        <v>238</v>
+        <v>92</v>
       </c>
       <c r="BM5" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BN5" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="BO5" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP5" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="BO5" s="15" t="s">
+      <c r="BQ5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR5" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="BP5" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="BQ5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="BR5" s="15" t="s">
-        <v>145</v>
-      </c>
       <c r="BS5" s="15" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="BT5" s="15" t="s">
-        <v>145</v>
+        <v>58</v>
       </c>
       <c r="BU5" s="15" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
       <c r="BV5" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="BW5" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="BX5" s="15" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="BY5" s="15" t="s">
         <v>16</v>
       </c>
       <c r="BZ5" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="CA5" s="15"/>
       <c r="CB5" s="15"/>
       <c r="CC5" s="15"/>
-      <c r="CD5" s="15"/>
+      <c r="CD5" s="13" t="s">
+        <v>203</v>
+      </c>
       <c r="CE5" s="15"/>
-      <c r="CF5" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="CG5" s="15" t="s">
-        <v>145</v>
-      </c>
+      <c r="CF5" s="15"/>
+      <c r="CG5" s="15"/>
       <c r="CH5" s="15" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="CI5" s="15" t="s">
-        <v>145</v>
+        <v>64</v>
       </c>
       <c r="CJ5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="CK5" s="15" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="CK5" s="15"/>
       <c r="CL5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="CM5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="CN5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="CO5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="CP5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="CQ5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="CR5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="CS5" s="15" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="CT5" s="15" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="CU5" s="15" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="CV5" s="15" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="CW5" s="15" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="CX5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="CY5" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="CZ5" s="15" t="s">
         <v>38</v>
@@ -15214,89 +15232,91 @@
         <v>38</v>
       </c>
       <c r="DC5" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="DD5" s="15" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="DE5" s="15" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="DF5" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="DG5" s="15" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="DH5" s="15" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="DI5" s="15" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="DJ5" s="15" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="DK5" s="15" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="DL5" s="15" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="DM5" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="DN5" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="DO5" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="DO5" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="DP5" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="DQ5" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="DR5" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="DS5" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="DT5" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="DU5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="DV5" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="DV5" s="15" t="s">
-        <v>78</v>
-      </c>
       <c r="DW5" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="DX5" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="DY5" s="22" t="s">
-        <v>250</v>
+        <v>299</v>
+      </c>
+      <c r="DY5" s="8" t="s">
+        <v>288</v>
       </c>
       <c r="DZ5" s="18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="EA5" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="EB5" s="18"/>
-      <c r="EC5" s="18"/>
-      <c r="ED5" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="EE5" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="EB5" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="EC5" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="EF5" s="18"/>
+      <c r="ED5" s="18"/>
+      <c r="EE5" s="18"/>
+      <c r="EF5" s="18" t="s">
+        <v>255</v>
+      </c>
       <c r="EG5" s="18"/>
       <c r="EH5" s="18"/>
     </row>
@@ -15311,7 +15331,7 @@
   <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15362,13 +15382,13 @@
         <v>23</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I1" s="26" t="s">
         <v>13</v>
@@ -15377,16 +15397,16 @@
         <v>0</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M1" s="26" t="s">
         <v>36</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O1" s="26" t="s">
         <v>39</v>
@@ -15398,19 +15418,19 @@
         <v>41</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="S1" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T1" s="26" t="s">
         <v>42</v>
       </c>
       <c r="U1" s="26" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="V1" s="26" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="W1" s="26" t="s">
         <v>43</v>
@@ -15431,31 +15451,31 @@
         <v>48</v>
       </c>
       <c r="AC1" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD1" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AE1" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AF1" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="AF1" s="26" t="s">
-        <v>98</v>
-      </c>
       <c r="AG1" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH1" s="26" t="s">
         <v>75</v>
-      </c>
-      <c r="AH1" s="26" t="s">
-        <v>76</v>
       </c>
       <c r="AI1" s="35" t="s">
         <v>24</v>
       </c>
       <c r="AJ1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AK1" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row customFormat="1" ht="25.5" r="2" s="7" spans="1:37">
@@ -15466,7 +15486,7 @@
         <v>34</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>31</v>
@@ -15477,38 +15497,38 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
       <c r="H2" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="K2" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>121</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>123</v>
       </c>
       <c r="M2" s="31" t="s">
         <v>37</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P2" s="32"/>
       <c r="Q2" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="R2" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S2" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T2" s="32" t="s">
         <v>67</v>
@@ -15517,49 +15537,49 @@
         <v>16</v>
       </c>
       <c r="V2" s="32" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="W2" s="31" t="s">
-        <v>100</v>
+        <v>289</v>
       </c>
       <c r="X2" s="31" t="s">
-        <v>68</v>
+        <v>290</v>
       </c>
       <c r="Y2" s="33" t="s">
-        <v>70</v>
+        <v>291</v>
       </c>
       <c r="Z2" s="31" t="s">
         <v>19</v>
       </c>
       <c r="AA2" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB2" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC2" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AD2" s="34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AE2" s="31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AF2" s="31" t="s">
         <v>60</v>
       </c>
       <c r="AG2" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH2" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="AH2" s="32" t="s">
-        <v>78</v>
-      </c>
       <c r="AI2" s="36" t="s">
-        <v>112</v>
+        <v>240</v>
       </c>
       <c r="AJ2" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AK2" s="36"/>
     </row>
@@ -15594,162 +15614,222 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>195</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="19.5" r="2" s="43" spans="1:7">
       <c r="A2" s="41" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>290</v>
-      </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+        <v>284</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="46.5" r="3" s="43" spans="1:7">
       <c r="A3" s="41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>289</v>
-      </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+        <v>284</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="34.5" r="4" s="43" spans="1:7">
       <c r="A4" s="41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>289</v>
-      </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+        <v>284</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row customFormat="1" r="5" s="43" spans="1:7">
       <c r="A5" s="41">
         <v>91127</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>289</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
+        <v>284</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row customFormat="1" r="6" s="43" spans="1:7">
       <c r="A6" s="41">
         <v>91127</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>289</v>
-      </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
+        <v>284</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row ht="45" r="7" spans="1:7">
       <c r="A7" s="49" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>289</v>
-      </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+        <v>284</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row ht="45" r="8" spans="1:7">
       <c r="A8" s="46">
         <v>91851</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>289</v>
-      </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+        <v>284</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row ht="45" r="9" spans="1:7">
       <c r="A9" s="46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>289</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+        <v>284</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row ht="45" r="10" spans="1:7">
       <c r="A10" s="46">
         <v>91853</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+        <v>284</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row ht="45" r="11" spans="1:7">
       <c r="A11" s="46">
         <v>91150</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+        <v>285</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>285</v>
+      </c>
       <c r="G11" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row ht="45" r="12" spans="1:7">
@@ -15757,16 +15837,22 @@
         <v>91155</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+        <v>285</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>285</v>
+      </c>
       <c r="G12" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row ht="45" r="13" spans="1:7">
@@ -15774,16 +15860,22 @@
         <v>91155</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+        <v>285</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>285</v>
+      </c>
       <c r="G13" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row ht="45" r="14" spans="1:7">
@@ -15791,16 +15883,22 @@
         <v>91315</v>
       </c>
       <c r="B14" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="G14" s="50" t="s">
         <v>215</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="50" t="s">
-        <v>217</v>
       </c>
     </row>
     <row ht="45" r="15" spans="1:7">
@@ -15808,16 +15906,22 @@
         <v>91315</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
+        <v>285</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>285</v>
+      </c>
       <c r="G15" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Business Summary Screen completed
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="298">
   <si>
     <t>Class Code</t>
   </si>
@@ -810,12 +810,6 @@
     <t>$1,235</t>
   </si>
   <si>
-    <t>FCGA AUTM-726550805</t>
-  </si>
-  <si>
-    <t>FGFL0020334900</t>
-  </si>
-  <si>
     <t>FCGA AUTM-259003251</t>
   </si>
   <si>
@@ -912,15 +906,6 @@
     <t>33/33/34</t>
   </si>
   <si>
-    <t>FCGA AUTM-628262323</t>
-  </si>
-  <si>
-    <t>BGFL0020336500</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-060914723</t>
-  </si>
-  <si>
     <t>FCGA AUTM-570803675</t>
   </si>
   <si>
@@ -937,6 +922,12 @@
   </si>
   <si>
     <t>$3,796</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-457799314</t>
+  </si>
+  <si>
+    <t>04/16/2020</t>
   </si>
 </sst>
 </file>
@@ -13281,8 +13272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EI5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="DX1" workbookViewId="0">
+      <selection activeCell="ED10" sqref="ED10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13633,70 +13624,70 @@
         <v>167</v>
       </c>
       <c r="CJ1" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="CK1" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="CL1" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="CK1" s="20" t="s">
+      <c r="CM1" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="CL1" s="20" t="s">
+      <c r="CN1" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="CM1" s="20" t="s">
+      <c r="CO1" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="CN1" s="20" t="s">
+      <c r="CP1" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="CO1" s="20" t="s">
+      <c r="CQ1" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="CP1" s="20" t="s">
+      <c r="CR1" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="CQ1" s="20" t="s">
+      <c r="CS1" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="CR1" s="20" t="s">
+      <c r="CT1" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="CS1" s="20" t="s">
+      <c r="CU1" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="CT1" s="20" t="s">
+      <c r="CV1" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="CU1" s="20" t="s">
+      <c r="CW1" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="CV1" s="20" t="s">
+      <c r="CX1" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="CY1" s="47" t="s">
         <v>275</v>
       </c>
-      <c r="CW1" s="20" t="s">
+      <c r="CZ1" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA1" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="DB1" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="DC1" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="CX1" s="47" t="s">
-        <v>286</v>
-      </c>
-      <c r="CY1" s="47" t="s">
+      <c r="DD1" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="CZ1" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="DA1" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="DB1" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="DC1" s="20" t="s">
+      <c r="DE1" s="20" t="s">
         <v>278</v>
-      </c>
-      <c r="DD1" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="DE1" s="20" t="s">
-        <v>280</v>
       </c>
       <c r="DF1" s="47" t="s">
         <v>168</v>
@@ -14152,13 +14143,13 @@
         <v>77</v>
       </c>
       <c r="DW2" s="12" t="s">
-        <v>110</v>
+        <v>240</v>
       </c>
       <c r="DX2" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="DY2" s="8" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="DZ2" s="18" t="s">
         <v>249</v>
@@ -14167,7 +14158,7 @@
         <v>250</v>
       </c>
       <c r="EB2" s="18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="EC2" s="18" t="s">
         <v>251</v>
@@ -14177,7 +14168,7 @@
       <c r="EF2" s="18"/>
       <c r="EG2" s="18"/>
       <c r="EH2" s="18" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row customHeight="1" ht="24" r="3" spans="1:138">
@@ -14543,10 +14534,10 @@
         <v>110</v>
       </c>
       <c r="DX3" s="12" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="DY3" s="22" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="DZ3" s="18" t="s">
         <v>249</v>
@@ -14565,7 +14556,7 @@
       <c r="EF3" s="18"/>
       <c r="EG3" s="18"/>
       <c r="EH3" s="18" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row customHeight="1" ht="24" r="4" spans="1:138">
@@ -14907,7 +14898,7 @@
         <v>240</v>
       </c>
       <c r="DX4" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="DY4" s="8" t="s">
         <v>248</v>
@@ -15295,10 +15286,10 @@
         <v>240</v>
       </c>
       <c r="DX5" s="12" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="DY5" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="DZ5" s="18" t="s">
         <v>249</v>
@@ -15307,7 +15298,7 @@
         <v>70</v>
       </c>
       <c r="EB5" s="18" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="EC5" s="18" t="s">
         <v>254</v>
@@ -15427,10 +15418,10 @@
         <v>42</v>
       </c>
       <c r="U1" s="26" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="V1" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W1" s="26" t="s">
         <v>43</v>
@@ -15540,13 +15531,13 @@
         <v>194</v>
       </c>
       <c r="W2" s="31" t="s">
+        <v>287</v>
+      </c>
+      <c r="X2" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y2" s="33" t="s">
         <v>289</v>
-      </c>
-      <c r="X2" s="31" t="s">
-        <v>290</v>
-      </c>
-      <c r="Y2" s="33" t="s">
-        <v>291</v>
       </c>
       <c r="Z2" s="31" t="s">
         <v>19</v>
@@ -15637,16 +15628,16 @@
         <v>81</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="46.5" r="3" s="43" spans="1:7">
@@ -15657,16 +15648,16 @@
         <v>160</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="34.5" r="4" s="43" spans="1:7">
@@ -15677,16 +15668,16 @@
         <v>82</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F4" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row customFormat="1" r="5" s="43" spans="1:7">
@@ -15697,16 +15688,16 @@
         <v>144</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row customFormat="1" r="6" s="43" spans="1:7">
@@ -15717,16 +15708,16 @@
         <v>159</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F6" s="45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row ht="45" r="7" spans="1:7">
@@ -15737,16 +15728,16 @@
         <v>162</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row ht="45" r="8" spans="1:7">
@@ -15757,16 +15748,16 @@
         <v>163</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row ht="45" r="9" spans="1:7">
@@ -15777,16 +15768,16 @@
         <v>190</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row ht="45" r="10" spans="1:7">
@@ -15797,16 +15788,16 @@
         <v>188</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row ht="45" r="11" spans="1:7">
@@ -15817,16 +15808,16 @@
         <v>208</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G11" s="50" t="s">
         <v>215</v>
@@ -15840,16 +15831,16 @@
         <v>209</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G12" s="50" t="s">
         <v>215</v>
@@ -15863,16 +15854,16 @@
         <v>208</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G13" s="50" t="s">
         <v>215</v>
@@ -15886,16 +15877,16 @@
         <v>213</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G14" s="50" t="s">
         <v>215</v>
@@ -15909,16 +15900,16 @@
         <v>214</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G15" s="50" t="s">
         <v>215</v>

</xml_diff>

<commit_message>
WC is working as Expected
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="380">
   <si>
     <t>Class Code</t>
   </si>
@@ -1050,9 +1050,6 @@
     <t>Hello</t>
   </si>
   <si>
-    <t>FCGA AUTM-023688551</t>
-  </si>
-  <si>
     <t>FWDE0020340000</t>
   </si>
   <si>
@@ -1173,61 +1170,10 @@
     <t>UWModify Total Incurred</t>
   </si>
   <si>
-    <t>FCGA AUTM-039420988</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-509979373</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-793554603</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-052381867</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-649286703</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-077157356</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-999160743</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-342865424</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-663337099</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-181099052</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-904382177</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-201482338</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-991942723</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-116745618</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-484859650</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-446539989</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-946504667</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-850426191</t>
-  </si>
-  <si>
-    <t>FCGA AUTM-542481200</t>
+    <t>FCGA AUTM-497908182</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-430194501</t>
   </si>
 </sst>
 </file>
@@ -13666,8 +13612,7 @@
     <col min="129" max="129" customWidth="true" style="24" width="30.5703125" collapsed="true"/>
     <col min="130" max="130" customWidth="true" width="21.7109375" collapsed="true"/>
     <col min="131" max="131" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="132" max="135" customWidth="true" style="24" width="24.85546875" collapsed="true"/>
-    <col min="136" max="136" customWidth="true" style="24" width="24.85546875" collapsed="true"/>
+    <col min="132" max="136" customWidth="true" style="24" width="24.85546875" collapsed="true"/>
     <col min="137" max="137" customWidth="true" style="2" width="14.0" collapsed="true"/>
     <col min="138" max="138" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
     <col min="139" max="139" customWidth="true" style="1" width="13.140625" collapsed="true"/>
@@ -14090,7 +14035,7 @@
         <v>212</v>
       </c>
       <c r="EF1" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="EG1" s="11" t="s">
         <v>16</v>
@@ -14531,7 +14476,7 @@
         <v>213</v>
       </c>
       <c r="EF2" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="EG2" s="15" t="s">
         <v>48</v>
@@ -14934,7 +14879,7 @@
         <v>213</v>
       </c>
       <c r="EF3" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="EG3" s="15" t="s">
         <v>49</v>
@@ -15313,7 +15258,7 @@
         <v>213</v>
       </c>
       <c r="EF4" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="EG4" s="15" t="s">
         <v>48</v>
@@ -15716,7 +15661,7 @@
         <v>213</v>
       </c>
       <c r="EF5" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="EG5" s="15" t="s">
         <v>48</v>
@@ -15766,8 +15711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="AU13" sqref="AU13"/>
+    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
+      <selection sqref="A1:BX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15796,8 +15741,7 @@
     <col min="31" max="43" customWidth="true" style="24" width="21.5703125" collapsed="true"/>
     <col min="44" max="44" customWidth="true" width="16.85546875" collapsed="true"/>
     <col min="45" max="45" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="46" max="50" customWidth="true" style="24" width="18.28515625" collapsed="true"/>
-    <col min="51" max="52" customWidth="true" style="24" width="18.28515625" collapsed="true"/>
+    <col min="46" max="52" customWidth="true" style="24" width="18.28515625" collapsed="true"/>
     <col min="53" max="53" customWidth="true" style="24" width="14.5703125" collapsed="true"/>
     <col min="54" max="56" customWidth="true" style="24" width="15.42578125" collapsed="true"/>
     <col min="57" max="57" customWidth="true" style="24" width="10.42578125" collapsed="true"/>
@@ -15950,10 +15894,10 @@
         <v>314</v>
       </c>
       <c r="AP1" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="AQ1" s="27" t="s">
         <v>342</v>
-      </c>
-      <c r="AQ1" s="27" t="s">
-        <v>343</v>
       </c>
       <c r="AR1" s="26" t="s">
         <v>95</v>
@@ -15961,32 +15905,32 @@
       <c r="AS1" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="AT1" s="35" t="s">
+      <c r="AT1" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="AU1" s="55" t="s">
+        <v>343</v>
+      </c>
+      <c r="AV1" s="35" t="s">
         <v>332</v>
       </c>
-      <c r="AU1" s="35" t="s">
+      <c r="AW1" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="AV1" s="35" t="s">
+      <c r="AX1" s="35" t="s">
         <v>334</v>
       </c>
-      <c r="AW1" s="35" t="s">
+      <c r="AY1" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="AX1" s="35" t="s">
+      <c r="AZ1" s="35" t="s">
         <v>336</v>
       </c>
-      <c r="AY1" s="26" t="s">
-        <v>340</v>
-      </c>
-      <c r="AZ1" s="55" t="s">
+      <c r="BA1" s="51" t="s">
         <v>344</v>
       </c>
-      <c r="BA1" s="51" t="s">
+      <c r="BB1" s="51" t="s">
         <v>345</v>
-      </c>
-      <c r="BB1" s="51" t="s">
-        <v>346</v>
       </c>
       <c r="BC1" s="51" t="s">
         <v>215</v>
@@ -15995,100 +15939,100 @@
         <v>214</v>
       </c>
       <c r="BE1" s="52" t="s">
+        <v>346</v>
+      </c>
+      <c r="BF1" s="53" t="s">
         <v>347</v>
       </c>
-      <c r="BF1" s="53" t="s">
+      <c r="BG1" s="35" t="s">
         <v>348</v>
       </c>
-      <c r="BG1" s="35" t="s">
+      <c r="BH1" s="35" t="s">
         <v>349</v>
       </c>
-      <c r="BH1" s="35" t="s">
+      <c r="BI1" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="BI1" s="35" t="s">
+      <c r="BJ1" s="35" t="s">
         <v>351</v>
       </c>
-      <c r="BJ1" s="35" t="s">
+      <c r="BK1" s="35" t="s">
         <v>352</v>
       </c>
-      <c r="BK1" s="35" t="s">
+      <c r="BL1" s="35" t="s">
         <v>353</v>
       </c>
-      <c r="BL1" s="35" t="s">
+      <c r="BM1" s="35" t="s">
         <v>354</v>
       </c>
-      <c r="BM1" s="35" t="s">
+      <c r="BN1" s="35" t="s">
         <v>355</v>
       </c>
-      <c r="BN1" s="35" t="s">
+      <c r="BO1" s="35" t="s">
         <v>356</v>
       </c>
-      <c r="BO1" s="35" t="s">
+      <c r="BP1" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="BP1" s="35" t="s">
+      <c r="BQ1" s="35" t="s">
         <v>358</v>
       </c>
-      <c r="BQ1" s="35" t="s">
+      <c r="BR1" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="BR1" s="35" t="s">
+      <c r="BS1" s="35" t="s">
         <v>360</v>
       </c>
-      <c r="BS1" s="35" t="s">
+      <c r="BT1" s="35" t="s">
         <v>361</v>
       </c>
-      <c r="BT1" s="35" t="s">
+      <c r="BU1" s="35" t="s">
         <v>362</v>
       </c>
-      <c r="BU1" s="35" t="s">
+      <c r="BV1" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="BV1" s="35" t="s">
+      <c r="BW1" s="35" t="s">
         <v>364</v>
       </c>
-      <c r="BW1" s="35" t="s">
+      <c r="BX1" s="35" t="s">
+        <v>366</v>
+      </c>
+      <c r="BY1" s="54" t="s">
         <v>365</v>
       </c>
-      <c r="BX1" s="35" t="s">
+      <c r="BZ1" s="54" t="s">
         <v>367</v>
       </c>
-      <c r="BY1" s="54" t="s">
-        <v>366</v>
-      </c>
-      <c r="BZ1" s="54" t="s">
+      <c r="CA1" s="54" t="s">
         <v>368</v>
       </c>
-      <c r="CA1" s="54" t="s">
+      <c r="CB1" s="54" t="s">
         <v>369</v>
       </c>
-      <c r="CB1" s="54" t="s">
+      <c r="CC1" s="54" t="s">
         <v>370</v>
       </c>
-      <c r="CC1" s="54" t="s">
+      <c r="CD1" s="54" t="s">
         <v>371</v>
       </c>
-      <c r="CD1" s="54" t="s">
+      <c r="CE1" s="54" t="s">
         <v>372</v>
       </c>
-      <c r="CE1" s="54" t="s">
+      <c r="CF1" s="54" t="s">
         <v>373</v>
       </c>
-      <c r="CF1" s="54" t="s">
+      <c r="CG1" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="CG1" s="54" t="s">
+      <c r="CH1" s="54" t="s">
         <v>375</v>
       </c>
-      <c r="CH1" s="54" t="s">
+      <c r="CI1" s="54" t="s">
         <v>376</v>
       </c>
-      <c r="CI1" s="54" t="s">
+      <c r="CJ1" s="54" t="s">
         <v>377</v>
-      </c>
-      <c r="CJ1" s="54" t="s">
-        <v>378</v>
       </c>
       <c r="CK1" s="26" t="s">
         <v>73</v>
@@ -16227,25 +16171,25 @@
         <v>59</v>
       </c>
       <c r="AT2" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="AU2" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV2" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="AU2" s="31" t="s">
+      <c r="AW2" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="AV2" s="31" t="s">
+      <c r="AX2" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="AW2" s="31" t="s">
+      <c r="AY2" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="AX2" s="31" t="s">
+      <c r="AZ2" s="31" t="s">
         <v>337</v>
-      </c>
-      <c r="AY2" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="AZ2" s="31" t="s">
-        <v>15</v>
       </c>
       <c r="BA2" s="29"/>
       <c r="BB2" s="29"/>
@@ -16349,10 +16293,10 @@
         <v>236</v>
       </c>
       <c r="CN2" s="36" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="CO2" s="36" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OK- Working Fine WC
</commit_message>
<xml_diff>
--- a/Smoke Test Data.xlsx
+++ b/Smoke Test Data.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="TD_GL" sheetId="1" r:id="rId1"/>
-    <sheet name="TD_WC" sheetId="2" r:id="rId2"/>
-    <sheet name="All States" sheetId="5" r:id="rId3"/>
-    <sheet name="TD_CSQ" sheetId="4" r:id="rId4"/>
+    <sheet name="TD_GL" r:id="rId1" sheetId="1"/>
+    <sheet name="TD_WC" r:id="rId2" sheetId="2"/>
+    <sheet name="All States" r:id="rId3" sheetId="5"/>
+    <sheet name="TD_CSQ" r:id="rId4" sheetId="4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TD_WC!$A$1:$CS$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">TD_WC!$A$1:$CS$24</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="646">
   <si>
     <t>TC ID</t>
   </si>
@@ -1906,6 +1906,60 @@
   </si>
   <si>
     <t>FCGA AUTM-408519817</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-421689610</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-540757820</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-511625540</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-602524356</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-340997655</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-943772730</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-528165060</t>
+  </si>
+  <si>
+    <t>FWLA0020604700</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-376010569</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-014202307</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-484056055</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-082486439</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-209622417</t>
+  </si>
+  <si>
+    <t>FWLA0020605000</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-798296536</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-311060886</t>
+  </si>
+  <si>
+    <t>FCGA AUTM-166417318</t>
   </si>
 </sst>
 </file>
@@ -2128,197 +2182,197 @@
     </border>
   </borders>
   <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="165"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="64">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="2" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="5" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="6" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="3" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="3" numFmtId="49" xfId="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="3" numFmtId="49" xfId="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="7" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="5" fontId="6" numFmtId="1" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="4" fontId="6" numFmtId="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="3">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="4">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="49" quotePrefix="1" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="9" fontId="10" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="9" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="9" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="8" fontId="9" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="8" fontId="9" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="8" fontId="9" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 10" xfId="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2 2" xfId="3"/>
     <cellStyle name="Normal 3 2 2" xfId="4"/>
     <cellStyle name="Normal 4 2 11" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2335,10 +2389,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2373,7 +2427,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2408,7 +2462,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2496,7 +2550,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -2505,13 +2559,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2521,7 +2575,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2530,7 +2584,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2539,7 +2593,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2549,12 +2603,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -2585,7 +2639,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -2604,7 +2658,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -2616,8 +2670,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FC13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:FD13"/>
   <sheetViews>
     <sheetView topLeftCell="EH1" workbookViewId="0">
       <selection activeCell="ES8" sqref="ES8"/>
@@ -2625,17 +2679,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="86" max="86" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="87" max="87" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="112" max="112" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="113" max="113" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="59" max="59" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="65" max="65" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="86" max="86" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="87" max="87" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="112" max="112" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="113" max="113" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3114,7 +3168,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="2" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -3469,7 +3523,7 @@
       <c r="FB2" s="18"/>
       <c r="FC2" s="18"/>
     </row>
-    <row r="3" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="3" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -3824,7 +3878,7 @@
       <c r="FB3" s="18"/>
       <c r="FC3" s="18"/>
     </row>
-    <row r="4" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="4" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -4193,7 +4247,7 @@
       <c r="FB4" s="18"/>
       <c r="FC4" s="18"/>
     </row>
-    <row r="5" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="5" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -4562,7 +4616,7 @@
       </c>
       <c r="FC5" s="18"/>
     </row>
-    <row r="6" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="6" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -4917,7 +4971,7 @@
       <c r="FB6" s="18"/>
       <c r="FC6" s="18"/>
     </row>
-    <row r="7" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="7" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -5272,7 +5326,7 @@
       <c r="FB7" s="18"/>
       <c r="FC7" s="18"/>
     </row>
-    <row r="8" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="8" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -5619,7 +5673,7 @@
       <c r="FB8" s="18"/>
       <c r="FC8" s="18"/>
     </row>
-    <row r="9" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="9" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -5966,7 +6020,7 @@
       <c r="FB9" s="18"/>
       <c r="FC9" s="18"/>
     </row>
-    <row r="10" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="10" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -6323,7 +6377,7 @@
       <c r="FB10" s="18"/>
       <c r="FC10" s="18"/>
     </row>
-    <row r="11" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="11" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -6680,7 +6734,7 @@
       <c r="FB11" s="18"/>
       <c r="FC11" s="18"/>
     </row>
-    <row r="12" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="12" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -7047,7 +7101,7 @@
       <c r="FB12" s="18"/>
       <c r="FC12" s="18"/>
     </row>
-    <row r="13" spans="1:159" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="24" r="13" s="8" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -7415,14 +7469,14 @@
       <c r="FC13" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CS24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CT24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I24"/>
@@ -7430,16 +7484,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15" style="33" collapsed="1"/>
-    <col min="3" max="3" width="24.5703125" style="33" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="15" style="33" collapsed="1"/>
-    <col min="11" max="11" width="40.85546875" style="33" customWidth="1" collapsed="1"/>
-    <col min="12" max="19" width="15" style="33" collapsed="1"/>
-    <col min="20" max="20" width="23.140625" style="33" customWidth="1" collapsed="1"/>
-    <col min="21" max="16384" width="15" style="33" collapsed="1"/>
+    <col min="1" max="2" style="33" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="33" width="24.5703125" collapsed="true"/>
+    <col min="4" max="10" style="33" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="33" width="40.85546875" collapsed="true"/>
+    <col min="12" max="19" style="33" width="15.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="33" width="23.140625" collapsed="true"/>
+    <col min="21" max="16384" style="33" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="32" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -7732,7 +7786,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="2" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A2" s="47">
         <v>1</v>
       </c>
@@ -7902,16 +7956,16 @@
       <c r="CO2" s="20"/>
       <c r="CP2" s="20"/>
       <c r="CQ2" s="21" t="s">
-        <v>204</v>
+        <v>634</v>
       </c>
       <c r="CR2" s="21" t="s">
-        <v>613</v>
+        <v>645</v>
       </c>
       <c r="CS2" s="21" t="s">
-        <v>205</v>
+        <v>642</v>
       </c>
     </row>
-    <row r="3" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="3" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A3" s="47">
         <v>2</v>
       </c>
@@ -8084,13 +8138,13 @@
         <v>204</v>
       </c>
       <c r="CR3" s="21" t="s">
-        <v>614</v>
+        <v>643</v>
       </c>
       <c r="CS3" s="21" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="4" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A4" s="47">
         <v>3</v>
       </c>
@@ -8269,7 +8323,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="5" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A5" s="47">
         <v>4</v>
       </c>
@@ -8448,7 +8502,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="6" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A6" s="47">
         <v>5</v>
       </c>
@@ -8627,7 +8681,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="7" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A7" s="47">
         <v>6</v>
       </c>
@@ -8806,7 +8860,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="8" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A8" s="47">
         <v>7</v>
       </c>
@@ -8985,7 +9039,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="9" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A9" s="47">
         <v>8</v>
       </c>
@@ -9164,7 +9218,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="10" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A10" s="47">
         <v>9</v>
       </c>
@@ -9343,7 +9397,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="11" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A11" s="47">
         <v>10</v>
       </c>
@@ -9522,7 +9576,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="12" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A12" s="47">
         <v>11</v>
       </c>
@@ -9701,7 +9755,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="13" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A13" s="47">
         <v>12</v>
       </c>
@@ -9880,7 +9934,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="14" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A14" s="47">
         <v>13</v>
       </c>
@@ -10059,7 +10113,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="15" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A15" s="47">
         <v>14</v>
       </c>
@@ -10238,7 +10292,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="16" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A16" s="47">
         <v>15</v>
       </c>
@@ -10417,7 +10471,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="17" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A17" s="47">
         <v>16</v>
       </c>
@@ -10596,7 +10650,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="18" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A18" s="47">
         <v>17</v>
       </c>
@@ -10775,7 +10829,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="19" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A19" s="47">
         <v>18</v>
       </c>
@@ -10954,7 +11008,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="20" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A20" s="47">
         <v>19</v>
       </c>
@@ -11133,7 +11187,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="21" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A21" s="47">
         <v>20</v>
       </c>
@@ -11312,7 +11366,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="22" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A22" s="47">
         <v>21</v>
       </c>
@@ -11491,7 +11545,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="23" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A23" s="47">
         <v>22</v>
       </c>
@@ -11670,7 +11724,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:97" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="25.5" r="24" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A24" s="47">
         <v>23</v>
       </c>
@@ -11851,14 +11905,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:CS24"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
@@ -11866,7 +11920,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.42578125" style="21" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" style="21" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -13278,13 +13332,13 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:HS15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
@@ -13292,16 +13346,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="228" max="16384" width="9.140625" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="61.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="228" max="16384" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="33" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>13</v>
       </c>
@@ -13321,7 +13375,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="19.5" r="2" s="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>330</v>
       </c>
@@ -13337,7 +13391,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="42" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="46.5" r="3" s="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>332</v>
       </c>
@@ -13353,7 +13407,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="42" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="34.5" r="4" s="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>334</v>
       </c>
@@ -13369,7 +13423,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>91127</v>
       </c>
@@ -13385,7 +13439,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>91127</v>
       </c>
@@ -13401,7 +13455,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
         <v>338</v>
       </c>
@@ -13417,7 +13471,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="45">
         <v>91851</v>
       </c>
@@ -13433,7 +13487,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>338</v>
       </c>
@@ -13449,7 +13503,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="45">
         <v>91853</v>
       </c>
@@ -13465,7 +13519,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="45">
         <v>91150</v>
       </c>
@@ -13481,7 +13535,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="45">
         <v>91155</v>
       </c>
@@ -13497,7 +13551,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="45">
         <v>91155</v>
       </c>
@@ -13513,7 +13567,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="45">
         <v>91315</v>
       </c>
@@ -13529,7 +13583,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="45">
         <v>91315</v>
       </c>
@@ -13546,7 +13600,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>